<commit_message>
update deqm R4 view
</commit_message>
<xml_diff>
--- a/docs/coverage-deqm.xlsx
+++ b/docs/coverage-deqm.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AP$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AP$44</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1689" uniqueCount="303">
   <si>
     <t>Path</t>
   </si>
@@ -125,13 +125,13 @@
     <t>Mapping: Quality Data Model</t>
   </si>
   <si>
-    <t>Mapping: Workflow Mapping</t>
+    <t>Mapping: Workflow Pattern</t>
   </si>
   <si>
     <t>Mapping: RIM Mapping</t>
   </si>
   <si>
-    <t>Mapping: W5 Mapping</t>
+    <t>Mapping: FiveWs Pattern Mapping</t>
   </si>
   <si>
     <t>Mapping: Canadian Dental Association eclaims standard</t>
@@ -161,17 +161,17 @@
     <t>This is the Coverage profile which is used to provide insurance information for scheduling an appointment and or registering a patient.</t>
   </si>
   <si>
+    <t>The Coverage resource contains the insurance card level information, which is customary to provide on claims and other communications between providers and insurers.</t>
+  </si>
+  <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}</t>
+dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.div.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}</t>
   </si>
   <si>
     <t>Participation</t>
   </si>
   <si>
     <t>Event</t>
-  </si>
-  <si>
-    <t>financial.support</t>
   </si>
   <si>
     <t>Coverage.id</t>
@@ -212,7 +212,7 @@
     <t>Metadata about the resource</t>
   </si>
   <si>
-    <t>The metadata about the resource. This is content that is maintained by the infrastructure. Changes to the content may not always be associated with version changes to the resource.</t>
+    <t>The metadata about the resource. This is content that is maintained by the infrastructure. Changes to the content might not always be associated with version changes to the resource.</t>
   </si>
   <si>
     <t>Resource.meta</t>
@@ -228,11 +228,10 @@
     <t>A set of rules under which this content was created</t>
   </si>
   <si>
-    <t>A reference to a set of rules that were followed when the resource was constructed, and which must be understood when processing the content.</t>
-  </si>
-  <si>
-    <t>Asserting this rule set restricts the content to be only understood by a limited set of trading partners. This inherently limits the usefulness of the data in the long term. However, the existing health eco-system is highly fractured, and not yet ready to define, collect, and exchange data in a generally computable sense. Wherever possible, implementers and/or specification writers should avoid using this element. 
-This element is labelled as a modifier because the implicit rules may provide additional knowledge about the resource that modifies it's meaning or interpretation.</t>
+    <t>A reference to a set of rules that were followed when the resource was constructed, and which must be understood when processing the content. Often, this is a reference to an implementation guide that defines the special rules along with other profiles etc.</t>
+  </si>
+  <si>
+    <t>Asserting this rule set restricts the content to be only understood by a limited set of trading partners. This inherently limits the usefulness of the data in the long term. However, the existing health eco-system is highly fractured, and not yet ready to define, collect, and exchange data in a generally computable sense. Wherever possible, implementers and/or specification writers should avoid using this element. Often, when used, the URL is a reference to an implementation guide that defines these special rules as part of it's narrative along with other profiles, value sets, etc.</t>
   </si>
   <si>
     <t>Resource.implicitRules</t>
@@ -251,10 +250,10 @@
     <t>The base language in which the resource is written.</t>
   </si>
   <si>
-    <t>Language is provided to support indexing and accessibility (typically, services such as text to speech use the language tag). The html language tag in the narrative applies  to the narrative. The language tag on the resource may be used to specify the language of other presentations generated from the data in the resource  Not all the content has to be in the base language. The Resource.language should not be assumed to apply to the narrative automatically. If a language is specified, it should it also be specified on the div element in the html (see rules in HTML5 for information about the relationship between xml:lang and the html lang attribute).</t>
-  </si>
-  <si>
-    <t>extensible</t>
+    <t>Language is provided to support indexing and accessibility (typically, services such as text to speech use the language tag). The html language tag in the narrative applies  to the narrative. The language tag on the resource may be used to specify the language of other presentations generated from the data in the resource. Not all the content has to be in the base language. The Resource.language should not be assumed to apply to the narrative automatically. If a language is specified, it should it also be specified on the div element in the html (see rules in HTML5 for information about the relationship between xml:lang and the html lang attribute).</t>
+  </si>
+  <si>
+    <t>preferred</t>
   </si>
   <si>
     <t>A human language.</t>
@@ -280,17 +279,13 @@
     <t>Text summary of the resource, for human interpretation</t>
   </si>
   <si>
-    <t>A human-readable narrative that contains a summary of the resource, and may be used to represent the content of the resource to a human. The narrative need not encode all the structured data, but is required to contain sufficient detail to make it "clinically safe" for a human to just read the narrative. Resource definitions may define what content should be represented in the narrative to ensure clinical safety.</t>
-  </si>
-  <si>
-    <t>Contained resources do not have narrative. Resources that are not contained SHOULD have a narrative. In some cases, a resource may only have text with little or no additional discrete data (as long as all minOccurs=1 elements are satisfied).  This may be necessary for data from legacy systems where information is captured as a "text blob" or where text is additionally entered raw or narrated and encoded in formation is added later.</t>
+    <t>A human-readable narrative that contains a summary of the resource and can be used to represent the content of the resource to a human. The narrative need not encode all the structured data, but is required to contain sufficient detail to make it "clinically safe" for a human to just read the narrative. Resource definitions may define what content should be represented in the narrative to ensure clinical safety.</t>
+  </si>
+  <si>
+    <t>Contained resources do not have narrative. Resources that are not contained SHOULD have a narrative. In some cases, a resource may only have text with little or no additional discrete data (as long as all minOccurs=1 elements are satisfied).  This may be necessary for data from legacy systems where information is captured as a "text blob" or where text is additionally entered raw or narrated and encoded information is added later.</t>
   </si>
   <si>
     <t>DomainResource.text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dom-1
-</t>
   </si>
   <si>
     <t>Act.text?</t>
@@ -313,7 +308,7 @@
     <t>These resources do not have an independent existence apart from the resource that contains them - they cannot be identified independently, and nor can they have their own independent transaction scope.</t>
   </si>
   <si>
-    <t>This should never be done when the content can be identified properly, as once identification is lost, it is extremely difficult (and context dependent) to restore it again.</t>
+    <t>This should never be done when the content can be identified properly, as once identification is lost, it is extremely difficult (and context dependent) to restore it again. Contained resources may have profiles and tags In their meta elements, but SHALL NOT have security labels.</t>
   </si>
   <si>
     <t>DomainResource.contained</t>
@@ -333,10 +328,10 @@
 </t>
   </si>
   <si>
-    <t>Additional Content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the resource. In order to make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+    <t>Additional content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the resource. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
   </si>
   <si>
     <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
@@ -351,7 +346,11 @@
     <t>Extensions that cannot be ignored</t>
   </si>
   <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the resource, and that modifies the understanding of the element that contains it. Usually modifier elements provide negation or qualification. In order to make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.</t>
+    <t>May be used to represent additional information that is not part of the basic definition of the resource and that modifies the understanding of the element that contains it and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
+Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
+  </si>
+  <si>
+    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
   </si>
   <si>
     <t>DomainResource.modifierExtension</t>
@@ -364,18 +363,27 @@
 </t>
   </si>
   <si>
-    <t>The primary coverage ID</t>
-  </si>
-  <si>
-    <t>The main (and possibly only) identifier for the coverage - often referred to as a Member Id, Certificate number, Personal Health Number or Case ID. May be constructed as the concatination of the Coverage.SubscriberID and the Coverage.dependant.</t>
-  </si>
-  <si>
-    <t>This value may uniquely identify the coverage or it may be used in conjunction with the additional identifiers below.</t>
+    <t>Business Identifier for the coverage</t>
+  </si>
+  <si>
+    <t>A unique identifier assigned to this coverage.</t>
+  </si>
+  <si>
+    <t>The main (and possibly only) identifier for the coverage - often referred to as a Member Id, Certificate number, Personal Health Number or Case ID. May be constructed as the concatenation of the Coverage.SubscriberID and the Coverage.dependant.</t>
+  </si>
+  <si>
+    <t>Allows coverages to be distinguished and referenced.</t>
   </si>
   <si>
     <t>Event.identifier</t>
   </si>
   <si>
+    <t>.id</t>
+  </si>
+  <si>
+    <t>FiveWs.identifier</t>
+  </si>
+  <si>
     <t>C02</t>
   </si>
   <si>
@@ -397,19 +405,25 @@
     <t>This element is labeled as a modifier because the status contains the code entered-in-error that marks the coverage as not currently valid.</t>
   </si>
   <si>
+    <t>Need to track the status of the resource as 'draft' resources may undergo further edits while 'active' resources are immutable and may only have their status changed to 'cancelled'.</t>
+  </si>
+  <si>
     <t>required</t>
   </si>
   <si>
     <t>A code specifying the state of the resource instance.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/fm-status</t>
+    <t>http://hl7.org/fhir/ValueSet/fm-status|4.0.0</t>
   </si>
   <si>
     <t>Event.status</t>
   </si>
   <si>
-    <t>status</t>
+    <t>Act.status</t>
+  </si>
+  <si>
+    <t>FiveWs.status</t>
   </si>
   <si>
     <t>Coverage.type</t>
@@ -419,7 +433,7 @@
 </t>
   </si>
   <si>
-    <t>Type of coverage such as medical or accident</t>
+    <t>Coverage category such as medical or accident</t>
   </si>
   <si>
     <t>The type of coverage: social program, medical plan, accident coverage (workers compensation, auto), group health or payment by an individual or organization.</t>
@@ -437,7 +451,7 @@
     <t>code</t>
   </si>
   <si>
-    <t>class</t>
+    <t>FiveWs.class</t>
   </si>
   <si>
     <t>IN1-15</t>
@@ -453,10 +467,16 @@
     <t>Owner of the policy</t>
   </si>
   <si>
-    <t>The party who 'owns' the insurance policy,  may be an individual, corporation or the subscriber's employer.</t>
-  </si>
-  <si>
-    <t>who.focus</t>
+    <t>The party who 'owns' the insurance policy.</t>
+  </si>
+  <si>
+    <t>For example: may be an individual, corporation or the subscriber's employer.</t>
+  </si>
+  <si>
+    <t>This provides employer information in the case of Worker's Compensation and other policies.</t>
+  </si>
+  <si>
+    <t>FiveWs.subject</t>
   </si>
   <si>
     <t>D01 through D09</t>
@@ -481,6 +501,12 @@
     <t>The party who has signed-up for or 'owns' the contractual relationship to the policy or to whom the benefit of the policy for services rendered to them or their family is due.</t>
   </si>
   <si>
+    <t>May be self or a parent in the case of dependants.</t>
+  </si>
+  <si>
+    <t>This is the party who is entitled to the benfits under the policy.</t>
+  </si>
+  <si>
     <t>Coverage.subscriberId</t>
   </si>
   <si>
@@ -504,37 +530,61 @@
 </t>
   </si>
   <si>
-    <t>Plan Beneficiary</t>
-  </si>
-  <si>
-    <t>The party who benefits from the insurance coverage., the patient when services are provided.</t>
-  </si>
-  <si>
-    <t>While not required, this would usually be the US Core Patient Resource for which the MRP was performed.</t>
+    <t>Plan beneficiary</t>
+  </si>
+  <si>
+    <t>The party who benefits from the insurance coverage; the patient when products and/or services are provided.</t>
+  </si>
+  <si>
+    <t>This is the party who receives treatment for which the costs are reimbursed under the coverage.</t>
   </si>
   <si>
     <t>Event.subject</t>
   </si>
   <si>
+    <t>Coverage.dependent</t>
+  </si>
+  <si>
+    <t>Dependent number</t>
+  </si>
+  <si>
+    <t>A unique identifier for a dependent under the coverage.</t>
+  </si>
+  <si>
+    <t>Periodically the member number is constructed from the subscriberId and the dependant number.</t>
+  </si>
+  <si>
+    <t>For some coverages a single identifier is issued to the Subscriber and then a unique dependent number is issued to each beneficiary.</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>- No exact HL7 v2 equivalent concept seems to exist;</t>
+  </si>
+  <si>
     <t>Coverage.relationship</t>
   </si>
   <si>
-    <t>Beneficiary relationship to the Subscriber</t>
+    <t>Beneficiary relationship to the subscriber</t>
   </si>
   <si>
     <t>The relationship of beneficiary (patient) to the subscriber.</t>
   </si>
   <si>
-    <t>To determine relationship between the patient and the subscriber.</t>
-  </si>
-  <si>
-    <t>example</t>
-  </si>
-  <si>
-    <t>The relationship between the Policyholder and the Beneficiary (insured/covered party/patient).</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/policyholder-relationship</t>
+    <t>Typically, an individual uses policies which are theirs (relationship='self') before policies owned by others.</t>
+  </si>
+  <si>
+    <t>To determine relationship between the patient and the subscriber to determine coordination of benefits.</t>
+  </si>
+  <si>
+    <t>extensible</t>
+  </si>
+  <si>
+    <t>The relationship between the Subscriber and the Beneficiary (insured/covered party/patient).</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/subscriber-relationship</t>
   </si>
   <si>
     <t>C03</t>
@@ -553,13 +603,19 @@
     <t>Time period during which the coverage is in force. A missing start date indicates the start date isn't known, a missing end date means the coverage is continuing to be in force.</t>
   </si>
   <si>
+    <t>Some insurers require the submission of the coverage term.</t>
+  </si>
+  <si>
     <t>participationPeriod</t>
   </si>
   <si>
-    <t>Event.occurrence</t>
-  </si>
-  <si>
-    <t>when.done</t>
+    <t>Event.occurrence[x]</t>
+  </si>
+  <si>
+    <t>Act.effectiveTime</t>
+  </si>
+  <si>
+    <t>FiveWs.done[x]</t>
   </si>
   <si>
     <t>IN1-12 / IN1-13</t>
@@ -568,16 +624,20 @@
     <t>Coverage.payor</t>
   </si>
   <si>
-    <t>Identifier for the plan or agreement issuer</t>
-  </si>
-  <si>
-    <t>The program or plan underwriter or payor including both insurance and non-insurance agreements, such as patient-pay agreements. May provide multiple identifiers such as insurance company identifier or business identifier (BIN number).</t>
-  </si>
-  <si>
-    <t>Need to identify the issuer to target for processing and for coordination of benefit processing.</t>
-  </si>
-  <si>
-    <t>who.author</t>
+    <t>Issuer of the policy</t>
+  </si>
+  <si>
+    <t>The program or plan underwriter or payor including both insurance and non-insurance agreements, such as patient-pay agreements.</t>
+  </si>
+  <si>
+    <t>May provide multiple identifiers such as insurance company identifier or business identifier (BIN number).
+For selfpay it may provide multiple paying persons and/or organizations.</t>
+  </si>
+  <si>
+    <t>Need to identify the issuer to target for claim processing and for coordination of benefit processing.</t>
+  </si>
+  <si>
+    <t>FiveWs.author</t>
   </si>
   <si>
     <t>A05</t>
@@ -589,7 +649,7 @@
     <t>C.30</t>
   </si>
   <si>
-    <t>Coverage.grouping</t>
+    <t>Coverage.class</t>
   </si>
   <si>
     <t xml:space="preserve">BackboneElement
@@ -599,20 +659,26 @@
     <t>Additional coverage classifications</t>
   </si>
   <si>
-    <t>A suite of underwrite specific classifiers, for example may be used to identify a class of coverage or employer group, Policy, Plan.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
+    <t>A suite of underwriter specific classifiers.</t>
+  </si>
+  <si>
+    <t>For example may be used to identify a class of coverage or employer group, Policy, Plan.</t>
+  </si>
+  <si>
+    <t>The codes provided on the health card which identify or confirm the specific policy for the insurer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 </t>
   </si>
   <si>
-    <t>Coverage.grouping.id</t>
-  </si>
-  <si>
-    <t>xml:id (or equivalent in JSON)</t>
-  </si>
-  <si>
-    <t>unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+    <t>Coverage.class.id</t>
+  </si>
+  <si>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
   </si>
   <si>
     <t>Element.id</t>
@@ -621,35 +687,63 @@
     <t>n/a</t>
   </si>
   <si>
-    <t>Coverage.grouping.extension</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. In order to make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+    <t>Coverage.class.extension</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
   </si>
   <si>
     <t>Element.extension</t>
   </si>
   <si>
-    <t>Coverage.grouping.modifierExtension</t>
+    <t>Coverage.class.modifierExtension</t>
   </si>
   <si>
     <t>extensions
 user contentmodifiers</t>
   </si>
   <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element, and that modifies the understanding of the element that contains it. Usually modifier elements provide negation or qualification. In order to make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.</t>
+    <t>Extensions that cannot be ignored even if unrecognized</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element and that modifies the understanding of the element in which it is contained and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
+Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
   </si>
   <si>
     <t>BackboneElement.modifierExtension</t>
   </si>
   <si>
-    <t>Coverage.grouping.group</t>
-  </si>
-  <si>
-    <t>An identifier for the group</t>
-  </si>
-  <si>
-    <t>Identifies a style or collective of coverage issued by the underwriter, for example may be used to identify an employer group. May also be referred to as a Policy or Group ID.</t>
+    <t>Coverage.class.type</t>
+  </si>
+  <si>
+    <t>Type of class such as 'group' or 'plan'</t>
+  </si>
+  <si>
+    <t>The type of classification for which an insurer-specific class label or number and optional name is provided, for example may be used to identify a class of coverage or employer group, Policy, Plan.</t>
+  </si>
+  <si>
+    <t>The insurer issued label for a specific health card value.</t>
+  </si>
+  <si>
+    <t>The policy classifications, eg. Group, Plan, Class, etc.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/coverage-class</t>
+  </si>
+  <si>
+    <t>Coverage.class.value</t>
+  </si>
+  <si>
+    <t>Value associated with the type</t>
+  </si>
+  <si>
+    <t>The alphanumeric string value associated with the insurer issued label.</t>
+  </si>
+  <si>
+    <t>For example, the Group or Plan number.</t>
+  </si>
+  <si>
+    <t>The insurer issued label and value are necessary to identify the specific policy.</t>
   </si>
   <si>
     <t>C11 (Division,Section)</t>
@@ -661,148 +755,16 @@
     <t>C.31</t>
   </si>
   <si>
-    <t>Coverage.grouping.groupDisplay</t>
-  </si>
-  <si>
-    <t>Display text for an identifier for the group</t>
-  </si>
-  <si>
-    <t>A short description for the group.</t>
-  </si>
-  <si>
-    <t>Coverage.grouping.subGroup</t>
-  </si>
-  <si>
-    <t>An identifier for the subsection of the group</t>
-  </si>
-  <si>
-    <t>Identifies a style or collective of coverage issued by the underwriter, for example may be used to identify a subset of an employer group.</t>
-  </si>
-  <si>
-    <t>Coverage.grouping.subGroupDisplay</t>
-  </si>
-  <si>
-    <t>Display text for the subsection of the group</t>
-  </si>
-  <si>
-    <t>A short description for the subgroup.</t>
-  </si>
-  <si>
-    <t>Coverage.grouping.plan</t>
-  </si>
-  <si>
-    <t>An identifier for the plan</t>
-  </si>
-  <si>
-    <t>Identifies a style or collective of coverage issued by the underwriter, for example may be used to identify a collection of benefits provided to employees. May be referred to as a Section or Division ID.</t>
-  </si>
-  <si>
-    <t>C01</t>
-  </si>
-  <si>
-    <t>IN1-35</t>
-  </si>
-  <si>
-    <t>Coverage.grouping.planDisplay</t>
-  </si>
-  <si>
-    <t>Display text for the plan</t>
-  </si>
-  <si>
-    <t>A short description for the plan.</t>
-  </si>
-  <si>
-    <t>Coverage.grouping.subPlan</t>
-  </si>
-  <si>
-    <t>An identifier for the subsection of the plan</t>
-  </si>
-  <si>
-    <t>Identifies a sub-style or sub-collective of coverage issued by the underwriter, for example may be used to identify a subset of a collection of benefits provided to employees.</t>
-  </si>
-  <si>
-    <t>IN1-10</t>
-  </si>
-  <si>
-    <t>Coverage.grouping.subPlanDisplay</t>
-  </si>
-  <si>
-    <t>Display text for the subsection of the plan</t>
-  </si>
-  <si>
-    <t>A short description for the subplan.</t>
-  </si>
-  <si>
-    <t>Coverage.grouping.class</t>
-  </si>
-  <si>
-    <t>An identifier for the class</t>
-  </si>
-  <si>
-    <t>Identifies a style or collective of coverage issues by the underwriter, for example may be used to identify a class of coverage such as a level of deductables or co-payment.</t>
-  </si>
-  <si>
-    <t>Coverage.grouping.classDisplay</t>
-  </si>
-  <si>
-    <t>Display text for the class</t>
+    <t>Coverage.class.name</t>
+  </si>
+  <si>
+    <t>Human readable description of the type and value</t>
   </si>
   <si>
     <t>A short description for the class.</t>
   </si>
   <si>
-    <t>Coverage.grouping.subClass</t>
-  </si>
-  <si>
-    <t>An identifier for the subsection of the class</t>
-  </si>
-  <si>
-    <t>Identifies a sub-style or sub-collective of coverage issues by the underwriter, for example may be used to identify a subclass of coverage such as a sub-level of deductables or co-payment.</t>
-  </si>
-  <si>
-    <t>Coverage.grouping.subClassDisplay</t>
-  </si>
-  <si>
-    <t>Display text for the subsection of the subclass</t>
-  </si>
-  <si>
-    <t>A short description for the subclass.</t>
-  </si>
-  <si>
-    <t>Coverage.dependent</t>
-  </si>
-  <si>
-    <t>Dependent number</t>
-  </si>
-  <si>
-    <t>A unique identifier for a dependent under the coverage.</t>
-  </si>
-  <si>
-    <t>For some coverage a single identifier is issued to the Subscriber and a dependent number issued to each beneficiary.</t>
-  </si>
-  <si>
-    <t>C17</t>
-  </si>
-  <si>
-    <t>- No exact HL7 v2 equivalent concept seems to exist;</t>
-  </si>
-  <si>
-    <t>Coverage.sequence</t>
-  </si>
-  <si>
-    <t>The plan instance or sequence counter</t>
-  </si>
-  <si>
-    <t>An optional counter for a particular instance of the identified coverage which increments upon each renewal.</t>
-  </si>
-  <si>
-    <t>Some coverage, for example social plans, may be offered in short time increments, for example for a week or a month at a time, so while the rest of the plan details and identifiers may remain constant over time, the instance is incremented with each renewal and provided to the covered party on their 'card'.</t>
-  </si>
-  <si>
-    <t>D11</t>
-  </si>
-  <si>
-    <t>No HL7 v2 equivalent concept seems to exist</t>
+    <t>Used to provide a meaningful description in correspondence to the patient.</t>
   </si>
   <si>
     <t>Coverage.order</t>
@@ -815,7 +777,10 @@
     <t>Relative order of the coverage</t>
   </si>
   <si>
-    <t>The order of applicability of this coverage relative to other coverages which are currently inforce. Note, there may be gaps in the numbering and this does not imply primary, secondard etc. as the specific positioning of coverages depends upon the episode of care.</t>
+    <t>The order of applicability of this coverage relative to other coverages which are currently in force. Note, there may be gaps in the numbering and this does not imply primary, secondary etc. as the specific positioning of coverages depends upon the episode of care.</t>
+  </si>
+  <si>
+    <t>Used in managing the coordination of benefits.</t>
   </si>
   <si>
     <t>Coverage.network</t>
@@ -827,7 +792,148 @@
     <t>The insurer-specific identifier for the insurer-defined network of providers to which the beneficiary may seek treatment which will be covered at the 'in-network' rate, otherwise 'out of network' terms and conditions apply.</t>
   </si>
   <si>
+    <t>Used in referral for treatment and in claims processing.</t>
+  </si>
+  <si>
     <t>D10</t>
+  </si>
+  <si>
+    <t>Coverage.costToBeneficiary</t>
+  </si>
+  <si>
+    <t>CoPay
+DeductibleExceptions</t>
+  </si>
+  <si>
+    <t>Patient payments for services/products</t>
+  </si>
+  <si>
+    <t>A suite of codes indicating the cost category and associated amount which have been detailed in the policy and may have been  included on the health card.</t>
+  </si>
+  <si>
+    <t>For example by knowing the patient visit co-pay, the provider can collect the amount prior to undertaking treatment.</t>
+  </si>
+  <si>
+    <t>Required by providers to manage financial transaction with the patient.</t>
+  </si>
+  <si>
+    <t>Coverage.costToBeneficiary.id</t>
+  </si>
+  <si>
+    <t>Coverage.costToBeneficiary.extension</t>
+  </si>
+  <si>
+    <t>Coverage.costToBeneficiary.modifierExtension</t>
+  </si>
+  <si>
+    <t>Coverage.costToBeneficiary.type</t>
+  </si>
+  <si>
+    <t>Cost category</t>
+  </si>
+  <si>
+    <t>The category of patient centric costs associated with treatment.</t>
+  </si>
+  <si>
+    <t>For example visit, specialist visits, emergency, inpatient care, etc.</t>
+  </si>
+  <si>
+    <t>Needed to identify the category associated with the amount for the patient.</t>
+  </si>
+  <si>
+    <t>The types of services to which patient copayments are specified.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/coverage-copay-type</t>
+  </si>
+  <si>
+    <t>Coverage.costToBeneficiary.value[x]</t>
+  </si>
+  <si>
+    <t>Quantity {SimpleQuantity}
+Money</t>
+  </si>
+  <si>
+    <t>The amount or percentage due from the beneficiary</t>
+  </si>
+  <si>
+    <t>The amount due from the patient for the cost category.</t>
+  </si>
+  <si>
+    <t>Amount may be expressed as a percentage of the service/product cost or a fixed amount of currency.</t>
+  </si>
+  <si>
+    <t>Needed to identify the amount for the patient associated with the category.</t>
+  </si>
+  <si>
+    <t>Coverage.costToBeneficiary.exception</t>
+  </si>
+  <si>
+    <t>Exceptions for patient payments</t>
+  </si>
+  <si>
+    <t>A suite of codes indicating exceptions or reductions to patient costs and their effective periods.</t>
+  </si>
+  <si>
+    <t>Coverage.costToBeneficiary.exception.id</t>
+  </si>
+  <si>
+    <t>Coverage.costToBeneficiary.exception.extension</t>
+  </si>
+  <si>
+    <t>Coverage.costToBeneficiary.exception.modifierExtension</t>
+  </si>
+  <si>
+    <t>Coverage.costToBeneficiary.exception.type</t>
+  </si>
+  <si>
+    <t>Exception category</t>
+  </si>
+  <si>
+    <t>The code for the specific exception.</t>
+  </si>
+  <si>
+    <t>Needed to identify the exception associated with the amount for the patient.</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>The types of exceptions from the part or full value of financial obligations such as copays.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/coverage-financial-exception</t>
+  </si>
+  <si>
+    <t>Coverage.costToBeneficiary.exception.period</t>
+  </si>
+  <si>
+    <t>The effective period of the exception</t>
+  </si>
+  <si>
+    <t>The timeframe during when the exception is in force.</t>
+  </si>
+  <si>
+    <t>Needed to identify the applicable timeframe for the exception for the correct calculation of patient costs.</t>
+  </si>
+  <si>
+    <t>Coverage.subrogation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boolean
+</t>
+  </si>
+  <si>
+    <t>Reimbursement to insurer</t>
+  </si>
+  <si>
+    <t>When 'subrogation=true' this insurance instance has been included not for adjudication but to provide insurers with the details to recover costs.</t>
+  </si>
+  <si>
+    <t>Typically, automotive and worker's compensation policies would be flagged with 'subrogation=true' to enable healthcare payors to collect against accident claims.</t>
+  </si>
+  <si>
+    <t>See definition for when to be used.</t>
   </si>
   <si>
     <t>Coverage.contract</t>
@@ -841,6 +947,9 @@
   </si>
   <si>
     <t>The policy(s) which constitute this insurance coverage.</t>
+  </si>
+  <si>
+    <t>To reference the legally binding contract between the policy holder and the insurer.</t>
   </si>
   <si>
     <t>IN1-16, 18,  19</t>
@@ -992,7 +1101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AP41"/>
+  <dimension ref="A1:AP44"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1001,7 +1110,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="34.8046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="51.6015625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.45703125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
@@ -1031,15 +1140,15 @@
     <col min="28" max="28" width="18.84375" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="33.828125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="31" max="31" width="41.1484375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="28.43359375" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="28.0703125" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="26.6875" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="22.67578125" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="22.0078125" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="33.046875" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="54.171875" customWidth="true" bestFit="true"/>
     <col min="41" max="41" width="50.94140625" customWidth="true" bestFit="true"/>
     <col min="42" max="42" width="57.1640625" customWidth="true" bestFit="true"/>
@@ -1206,7 +1315,9 @@
       <c r="L2" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="M2" s="2"/>
+      <c r="M2" t="s" s="2">
+        <v>48</v>
+      </c>
       <c r="N2" s="2"/>
       <c r="O2" t="s" s="2">
         <v>43</v>
@@ -1267,19 +1378,19 @@
         <v>43</v>
       </c>
       <c r="AI2" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AJ2" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AK2" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AL2" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AM2" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AN2" t="s" s="2">
         <v>43</v>
@@ -1862,19 +1973,19 @@
         <v>53</v>
       </c>
       <c r="AH7" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI7" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AJ7" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK7" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AL7" t="s" s="2">
         <v>88</v>
-      </c>
-      <c r="AI7" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AJ7" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK7" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL7" t="s" s="2">
-        <v>89</v>
       </c>
       <c r="AM7" t="s" s="2">
         <v>43</v>
@@ -1891,11 +2002,11 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" t="s" s="2">
@@ -1914,16 +2025,16 @@
         <v>43</v>
       </c>
       <c r="J8" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="K8" t="s" s="2">
         <v>92</v>
       </c>
-      <c r="K8" t="s" s="2">
+      <c r="L8" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="L8" t="s" s="2">
+      <c r="M8" t="s" s="2">
         <v>94</v>
-      </c>
-      <c r="M8" t="s" s="2">
-        <v>95</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -1973,7 +2084,7 @@
         <v>43</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>44</v>
@@ -1994,7 +2105,7 @@
         <v>43</v>
       </c>
       <c r="AL8" t="s" s="2">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AM8" t="s" s="2">
         <v>43</v>
@@ -2011,11 +2122,11 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
@@ -2034,16 +2145,16 @@
         <v>43</v>
       </c>
       <c r="J9" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="K9" t="s" s="2">
         <v>100</v>
       </c>
-      <c r="K9" t="s" s="2">
+      <c r="L9" t="s" s="2">
         <v>101</v>
       </c>
-      <c r="L9" t="s" s="2">
+      <c r="M9" t="s" s="2">
         <v>102</v>
-      </c>
-      <c r="M9" t="s" s="2">
-        <v>103</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
@@ -2093,7 +2204,7 @@
         <v>43</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>44</v>
@@ -2114,7 +2225,7 @@
         <v>43</v>
       </c>
       <c r="AL9" t="s" s="2">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AM9" t="s" s="2">
         <v>43</v>
@@ -2131,11 +2242,11 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
@@ -2154,18 +2265,20 @@
         <v>43</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K10" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="L10" t="s" s="2">
         <v>106</v>
       </c>
-      <c r="L10" t="s" s="2">
+      <c r="M10" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="N10" t="s" s="2">
         <v>107</v>
       </c>
-      <c r="M10" t="s" s="2">
-        <v>103</v>
-      </c>
-      <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
         <v>43</v>
       </c>
@@ -2234,7 +2347,7 @@
         <v>43</v>
       </c>
       <c r="AL10" t="s" s="2">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AM10" t="s" s="2">
         <v>43</v>
@@ -2282,9 +2395,11 @@
       <c r="L11" t="s" s="2">
         <v>112</v>
       </c>
-      <c r="M11" s="2"/>
+      <c r="M11" t="s" s="2">
+        <v>113</v>
+      </c>
       <c r="N11" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="O11" t="s" s="2">
         <v>43</v>
@@ -2351,27 +2466,27 @@
         <v>43</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>43</v>
+        <v>116</v>
       </c>
       <c r="AM11" t="s" s="2">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="AN11" t="s" s="2">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AO11" t="s" s="2">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AP11" t="s" s="2">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -2379,7 +2494,7 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s" s="2">
         <v>53</v>
@@ -2397,15 +2512,17 @@
         <v>73</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>121</v>
-      </c>
-      <c r="N12" s="2"/>
+        <v>124</v>
+      </c>
+      <c r="N12" t="s" s="2">
+        <v>125</v>
+      </c>
       <c r="O12" t="s" s="2">
         <v>43</v>
       </c>
@@ -2429,13 +2546,13 @@
         <v>43</v>
       </c>
       <c r="W12" t="s" s="2">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="X12" t="s" s="2">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="Y12" t="s" s="2">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="Z12" t="s" s="2">
         <v>43</v>
@@ -2453,10 +2570,10 @@
         <v>43</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="AG12" t="s" s="2">
         <v>53</v>
@@ -2471,13 +2588,13 @@
         <v>43</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>43</v>
+        <v>130</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="AN12" t="s" s="2">
         <v>43</v>
@@ -2491,7 +2608,7 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -2514,17 +2631,17 @@
         <v>54</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" t="s" s="2">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="O13" t="s" s="2">
         <v>43</v>
@@ -2549,32 +2666,32 @@
         <v>43</v>
       </c>
       <c r="W13" t="s" s="2">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="X13" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="Y13" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="Z13" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA13" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB13" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC13" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD13" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE13" t="s" s="2">
         <v>132</v>
       </c>
-      <c r="Y13" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="Z13" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA13" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB13" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC13" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD13" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE13" t="s" s="2">
-        <v>127</v>
-      </c>
       <c r="AF13" t="s" s="2">
         <v>44</v>
       </c>
@@ -2588,7 +2705,7 @@
         <v>43</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="AK13" t="s" s="2">
         <v>43</v>
@@ -2597,13 +2714,13 @@
         <v>43</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="AN13" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AO13" t="s" s="2">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="AP13" t="s" s="2">
         <v>43</v>
@@ -2611,7 +2728,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -2634,16 +2751,20 @@
         <v>54</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>140</v>
-      </c>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
+        <v>145</v>
+      </c>
+      <c r="M14" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="N14" t="s" s="2">
+        <v>147</v>
+      </c>
       <c r="O14" t="s" s="2">
         <v>43</v>
       </c>
@@ -2691,7 +2812,7 @@
         <v>43</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>44</v>
@@ -2715,21 +2836,21 @@
         <v>43</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="AN14" t="s" s="2">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="AO14" t="s" s="2">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="AP14" t="s" s="2">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -2752,16 +2873,20 @@
         <v>54</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>148</v>
-      </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
+        <v>155</v>
+      </c>
+      <c r="M15" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="N15" t="s" s="2">
+        <v>157</v>
+      </c>
       <c r="O15" t="s" s="2">
         <v>43</v>
       </c>
@@ -2809,7 +2934,7 @@
         <v>43</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>44</v>
@@ -2833,21 +2958,21 @@
         <v>43</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="AO15" t="s" s="2">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="AP15" t="s" s="2">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2870,17 +2995,17 @@
         <v>54</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" t="s" s="2">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="O16" t="s" s="2">
         <v>43</v>
@@ -2929,45 +3054,45 @@
         <v>43</v>
       </c>
       <c r="AE16" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="AF16" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AG16" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AJ16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AL16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM16" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="AN16" t="s" s="2">
         <v>149</v>
       </c>
-      <c r="AF16" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG16" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AH16" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI16" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AJ16" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK16" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL16" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM16" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="AN16" t="s" s="2">
-        <v>142</v>
-      </c>
       <c r="AO16" t="s" s="2">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="AP16" t="s" s="2">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2975,7 +3100,7 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F17" t="s" s="2">
         <v>53</v>
@@ -2990,17 +3115,17 @@
         <v>54</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" t="s" s="2">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>43</v>
@@ -3049,10 +3174,10 @@
         <v>43</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>53</v>
@@ -3067,27 +3192,27 @@
         <v>43</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="AL17" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="AO17" t="s" s="2">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="AP17" t="s" s="2">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3107,20 +3232,22 @@
         <v>43</v>
       </c>
       <c r="I18" t="s" s="2">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>128</v>
+        <v>159</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>162</v>
-      </c>
-      <c r="M18" s="2"/>
+        <v>171</v>
+      </c>
+      <c r="M18" t="s" s="2">
+        <v>172</v>
+      </c>
       <c r="N18" t="s" s="2">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="O18" t="s" s="2">
         <v>43</v>
@@ -3145,13 +3272,13 @@
         <v>43</v>
       </c>
       <c r="W18" t="s" s="2">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="X18" t="s" s="2">
-        <v>165</v>
+        <v>43</v>
       </c>
       <c r="Y18" t="s" s="2">
-        <v>166</v>
+        <v>43</v>
       </c>
       <c r="Z18" t="s" s="2">
         <v>43</v>
@@ -3169,7 +3296,7 @@
         <v>43</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>44</v>
@@ -3196,10 +3323,10 @@
         <v>43</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="AO18" t="s" s="2">
-        <v>43</v>
+        <v>175</v>
       </c>
       <c r="AP18" t="s" s="2">
         <v>43</v>
@@ -3207,7 +3334,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3227,19 +3354,23 @@
         <v>43</v>
       </c>
       <c r="I19" t="s" s="2">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>169</v>
+        <v>133</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>171</v>
-      </c>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
+        <v>178</v>
+      </c>
+      <c r="M19" t="s" s="2">
+        <v>179</v>
+      </c>
+      <c r="N19" t="s" s="2">
+        <v>180</v>
+      </c>
       <c r="O19" t="s" s="2">
         <v>43</v>
       </c>
@@ -3263,13 +3394,13 @@
         <v>43</v>
       </c>
       <c r="W19" t="s" s="2">
-        <v>43</v>
+        <v>181</v>
       </c>
       <c r="X19" t="s" s="2">
-        <v>43</v>
+        <v>182</v>
       </c>
       <c r="Y19" t="s" s="2">
-        <v>43</v>
+        <v>183</v>
       </c>
       <c r="Z19" t="s" s="2">
         <v>43</v>
@@ -3287,7 +3418,7 @@
         <v>43</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>44</v>
@@ -3302,30 +3433,30 @@
         <v>43</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>172</v>
+        <v>43</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>173</v>
+        <v>43</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>174</v>
+        <v>43</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>43</v>
+        <v>184</v>
       </c>
       <c r="AO19" t="s" s="2">
-        <v>175</v>
+        <v>43</v>
       </c>
       <c r="AP19" t="s" s="2">
         <v>43</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3336,10 +3467,10 @@
         <v>44</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>43</v>
@@ -3348,17 +3479,17 @@
         <v>54</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>138</v>
+        <v>186</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" t="s" s="2">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>43</v>
@@ -3407,13 +3538,13 @@
         <v>43</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG20" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="AH20" t="s" s="2">
         <v>43</v>
@@ -3422,30 +3553,30 @@
         <v>43</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>43</v>
+        <v>190</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>43</v>
+        <v>191</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>43</v>
+        <v>192</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>181</v>
+        <v>43</v>
       </c>
       <c r="AO20" t="s" s="2">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="AP20" t="s" s="2">
-        <v>183</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="21" hidden="true">
+    <row r="21">
       <c r="A21" t="s" s="2">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3453,31 +3584,35 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F21" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>43</v>
       </c>
       <c r="I21" t="s" s="2">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>185</v>
+        <v>143</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
+        <v>197</v>
+      </c>
+      <c r="M21" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="N21" t="s" s="2">
+        <v>199</v>
+      </c>
       <c r="O21" t="s" s="2">
         <v>43</v>
       </c>
@@ -3525,19 +3660,19 @@
         <v>43</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="AG21" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="AH21" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>188</v>
+        <v>43</v>
       </c>
       <c r="AJ21" t="s" s="2">
         <v>43</v>
@@ -3549,21 +3684,21 @@
         <v>43</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>43</v>
+        <v>200</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>43</v>
+        <v>201</v>
       </c>
       <c r="AO21" t="s" s="2">
-        <v>43</v>
+        <v>202</v>
       </c>
       <c r="AP21" t="s" s="2">
-        <v>43</v>
+        <v>203</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3574,7 +3709,7 @@
         <v>44</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G22" t="s" s="2">
         <v>43</v>
@@ -3586,16 +3721,20 @@
         <v>43</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>150</v>
+        <v>205</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
+        <v>207</v>
+      </c>
+      <c r="M22" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="N22" t="s" s="2">
+        <v>209</v>
+      </c>
       <c r="O22" t="s" s="2">
         <v>43</v>
       </c>
@@ -3643,19 +3782,19 @@
         <v>43</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="AH22" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>43</v>
+        <v>210</v>
       </c>
       <c r="AJ22" t="s" s="2">
         <v>43</v>
@@ -3664,7 +3803,7 @@
         <v>43</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>193</v>
+        <v>43</v>
       </c>
       <c r="AM22" t="s" s="2">
         <v>43</v>
@@ -3681,18 +3820,18 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
         <v>44</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>43</v>
@@ -3704,17 +3843,15 @@
         <v>43</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>100</v>
+        <v>159</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>101</v>
+        <v>212</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>103</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
         <v>43</v>
@@ -3763,13 +3900,13 @@
         <v>43</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>196</v>
+        <v>214</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="AH23" t="s" s="2">
         <v>43</v>
@@ -3784,7 +3921,7 @@
         <v>43</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="AM23" t="s" s="2">
         <v>43</v>
@@ -3801,11 +3938,11 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>197</v>
+        <v>216</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>198</v>
+        <v>98</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
@@ -3818,22 +3955,22 @@
         <v>43</v>
       </c>
       <c r="H24" t="s" s="2">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J24" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="K24" t="s" s="2">
         <v>100</v>
       </c>
-      <c r="K24" t="s" s="2">
-        <v>106</v>
-      </c>
       <c r="L24" t="s" s="2">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
@@ -3883,7 +4020,7 @@
         <v>43</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>200</v>
+        <v>218</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>44</v>
@@ -3904,7 +4041,7 @@
         <v>43</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>97</v>
+        <v>215</v>
       </c>
       <c r="AM24" t="s" s="2">
         <v>43</v>
@@ -3921,39 +4058,43 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
         <v>44</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G25" t="s" s="2">
         <v>43</v>
       </c>
       <c r="H25" t="s" s="2">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="I25" t="s" s="2">
         <v>54</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>202</v>
+        <v>221</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
+        <v>222</v>
+      </c>
+      <c r="M25" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="N25" t="s" s="2">
+        <v>107</v>
+      </c>
       <c r="O25" t="s" s="2">
         <v>43</v>
       </c>
@@ -4001,13 +4142,13 @@
         <v>43</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>201</v>
+        <v>223</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG25" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="AH25" t="s" s="2">
         <v>43</v>
@@ -4022,24 +4163,24 @@
         <v>43</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="AM25" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>204</v>
+        <v>43</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>205</v>
+        <v>43</v>
       </c>
       <c r="AP25" t="s" s="2">
-        <v>206</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4047,7 +4188,7 @@
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F26" t="s" s="2">
         <v>53</v>
@@ -4062,16 +4203,18 @@
         <v>54</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>208</v>
+        <v>225</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
+      <c r="N26" t="s" s="2">
+        <v>227</v>
+      </c>
       <c r="O26" t="s" s="2">
         <v>43</v>
       </c>
@@ -4095,13 +4238,13 @@
         <v>43</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>43</v>
+        <v>181</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>43</v>
+        <v>228</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>43</v>
+        <v>229</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>43</v>
@@ -4119,10 +4262,10 @@
         <v>43</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>53</v>
@@ -4146,18 +4289,18 @@
         <v>43</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>204</v>
+        <v>43</v>
       </c>
       <c r="AO26" t="s" s="2">
-        <v>205</v>
+        <v>43</v>
       </c>
       <c r="AP26" t="s" s="2">
-        <v>206</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4165,7 +4308,7 @@
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F27" t="s" s="2">
         <v>53</v>
@@ -4180,16 +4323,20 @@
         <v>54</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
+        <v>232</v>
+      </c>
+      <c r="M27" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="N27" t="s" s="2">
+        <v>234</v>
+      </c>
       <c r="O27" t="s" s="2">
         <v>43</v>
       </c>
@@ -4237,10 +4384,10 @@
         <v>43</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>53</v>
@@ -4264,18 +4411,18 @@
         <v>43</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>43</v>
+        <v>235</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>205</v>
+        <v>236</v>
       </c>
       <c r="AP27" t="s" s="2">
-        <v>43</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>213</v>
+        <v>238</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4298,16 +4445,18 @@
         <v>54</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>214</v>
+        <v>239</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>215</v>
+        <v>240</v>
       </c>
       <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
+      <c r="N28" t="s" s="2">
+        <v>241</v>
+      </c>
       <c r="O28" t="s" s="2">
         <v>43</v>
       </c>
@@ -4355,7 +4504,7 @@
         <v>43</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>213</v>
+        <v>238</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>44</v>
@@ -4382,18 +4531,18 @@
         <v>43</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>43</v>
+        <v>235</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>205</v>
+        <v>236</v>
       </c>
       <c r="AP28" t="s" s="2">
-        <v>43</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>216</v>
+        <v>242</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4416,16 +4565,18 @@
         <v>54</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>150</v>
+        <v>243</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>217</v>
+        <v>244</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>218</v>
+        <v>245</v>
       </c>
       <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
+      <c r="N29" t="s" s="2">
+        <v>246</v>
+      </c>
       <c r="O29" t="s" s="2">
         <v>43</v>
       </c>
@@ -4473,7 +4624,7 @@
         <v>43</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>216</v>
+        <v>242</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>44</v>
@@ -4500,10 +4651,10 @@
         <v>43</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>219</v>
+        <v>43</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>220</v>
+        <v>175</v>
       </c>
       <c r="AP29" t="s" s="2">
         <v>43</v>
@@ -4511,7 +4662,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>221</v>
+        <v>247</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4534,16 +4685,18 @@
         <v>54</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>222</v>
+        <v>248</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>223</v>
+        <v>249</v>
       </c>
       <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
+      <c r="N30" t="s" s="2">
+        <v>250</v>
+      </c>
       <c r="O30" t="s" s="2">
         <v>43</v>
       </c>
@@ -4591,7 +4744,7 @@
         <v>43</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>221</v>
+        <v>247</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>44</v>
@@ -4618,10 +4771,10 @@
         <v>43</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>219</v>
+        <v>251</v>
       </c>
       <c r="AO30" t="s" s="2">
-        <v>220</v>
+        <v>43</v>
       </c>
       <c r="AP30" t="s" s="2">
         <v>43</v>
@@ -4629,18 +4782,18 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>224</v>
+        <v>252</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>43</v>
+        <v>253</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
         <v>44</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>43</v>
@@ -4649,19 +4802,23 @@
         <v>43</v>
       </c>
       <c r="I31" t="s" s="2">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>150</v>
+        <v>205</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>225</v>
+        <v>254</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
+        <v>255</v>
+      </c>
+      <c r="M31" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="N31" t="s" s="2">
+        <v>257</v>
+      </c>
       <c r="O31" t="s" s="2">
         <v>43</v>
       </c>
@@ -4709,19 +4866,19 @@
         <v>43</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>224</v>
+        <v>252</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG31" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="AH31" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>43</v>
+        <v>210</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>43</v>
@@ -4739,7 +4896,7 @@
         <v>43</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>227</v>
+        <v>43</v>
       </c>
       <c r="AP31" t="s" s="2">
         <v>43</v>
@@ -4747,7 +4904,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>228</v>
+        <v>258</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4767,16 +4924,16 @@
         <v>43</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -4827,7 +4984,7 @@
         <v>43</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>44</v>
@@ -4848,7 +5005,7 @@
         <v>43</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>43</v>
+        <v>215</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>43</v>
@@ -4857,7 +5014,7 @@
         <v>43</v>
       </c>
       <c r="AO32" t="s" s="2">
-        <v>227</v>
+        <v>43</v>
       </c>
       <c r="AP32" t="s" s="2">
         <v>43</v>
@@ -4865,18 +5022,18 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>231</v>
+        <v>259</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
         <v>44</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>43</v>
@@ -4885,18 +5042,20 @@
         <v>43</v>
       </c>
       <c r="I33" t="s" s="2">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>232</v>
+        <v>100</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>233</v>
-      </c>
-      <c r="M33" s="2"/>
+        <v>217</v>
+      </c>
+      <c r="M33" t="s" s="2">
+        <v>102</v>
+      </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>43</v>
@@ -4945,13 +5104,13 @@
         <v>43</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="AH33" t="s" s="2">
         <v>43</v>
@@ -4966,16 +5125,16 @@
         <v>43</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>43</v>
+        <v>215</v>
       </c>
       <c r="AM33" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>219</v>
+        <v>43</v>
       </c>
       <c r="AO33" t="s" s="2">
-        <v>220</v>
+        <v>43</v>
       </c>
       <c r="AP33" t="s" s="2">
         <v>43</v>
@@ -4983,39 +5142,43 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>234</v>
+        <v>260</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
         <v>44</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G34" t="s" s="2">
         <v>43</v>
       </c>
       <c r="H34" t="s" s="2">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="I34" t="s" s="2">
         <v>54</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
+        <v>222</v>
+      </c>
+      <c r="M34" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="N34" t="s" s="2">
+        <v>107</v>
+      </c>
       <c r="O34" t="s" s="2">
         <v>43</v>
       </c>
@@ -5063,13 +5226,13 @@
         <v>43</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG34" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="AH34" t="s" s="2">
         <v>43</v>
@@ -5084,16 +5247,16 @@
         <v>43</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>219</v>
+        <v>43</v>
       </c>
       <c r="AO34" t="s" s="2">
-        <v>220</v>
+        <v>43</v>
       </c>
       <c r="AP34" t="s" s="2">
         <v>43</v>
@@ -5101,7 +5264,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>237</v>
+        <v>261</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5124,16 +5287,20 @@
         <v>54</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
+        <v>263</v>
+      </c>
+      <c r="M35" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="N35" t="s" s="2">
+        <v>265</v>
+      </c>
       <c r="O35" t="s" s="2">
         <v>43</v>
       </c>
@@ -5157,13 +5324,13 @@
         <v>43</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>43</v>
+        <v>181</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>43</v>
+        <v>266</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>43</v>
+        <v>267</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>43</v>
@@ -5181,7 +5348,7 @@
         <v>43</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>237</v>
+        <v>261</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>44</v>
@@ -5208,10 +5375,10 @@
         <v>43</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>219</v>
+        <v>43</v>
       </c>
       <c r="AO35" t="s" s="2">
-        <v>220</v>
+        <v>43</v>
       </c>
       <c r="AP35" t="s" s="2">
         <v>43</v>
@@ -5219,7 +5386,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>240</v>
+        <v>268</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5227,7 +5394,7 @@
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F36" t="s" s="2">
         <v>53</v>
@@ -5242,16 +5409,20 @@
         <v>54</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>150</v>
+        <v>269</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>241</v>
+        <v>270</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
+        <v>271</v>
+      </c>
+      <c r="M36" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="N36" t="s" s="2">
+        <v>273</v>
+      </c>
       <c r="O36" t="s" s="2">
         <v>43</v>
       </c>
@@ -5299,10 +5470,10 @@
         <v>43</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>240</v>
+        <v>268</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>53</v>
@@ -5326,18 +5497,18 @@
         <v>43</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="AO36" t="s" s="2">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="AP36" t="s" s="2">
-        <v>43</v>
+        <v>237</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>243</v>
+        <v>274</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5348,7 +5519,7 @@
         <v>44</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>43</v>
@@ -5357,20 +5528,20 @@
         <v>43</v>
       </c>
       <c r="I37" t="s" s="2">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>150</v>
+        <v>205</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>244</v>
+        <v>275</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>245</v>
+        <v>276</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" t="s" s="2">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>43</v>
@@ -5419,19 +5590,19 @@
         <v>43</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>243</v>
+        <v>274</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="AH37" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>43</v>
+        <v>210</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>43</v>
@@ -5446,10 +5617,10 @@
         <v>43</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>247</v>
+        <v>43</v>
       </c>
       <c r="AO37" t="s" s="2">
-        <v>248</v>
+        <v>43</v>
       </c>
       <c r="AP37" t="s" s="2">
         <v>43</v>
@@ -5457,7 +5628,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>249</v>
+        <v>277</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5477,21 +5648,19 @@
         <v>43</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>250</v>
+        <v>212</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>251</v>
+        <v>213</v>
       </c>
       <c r="M38" s="2"/>
-      <c r="N38" t="s" s="2">
-        <v>252</v>
-      </c>
+      <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
         <v>43</v>
       </c>
@@ -5539,7 +5708,7 @@
         <v>43</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>44</v>
@@ -5560,16 +5729,16 @@
         <v>43</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>43</v>
+        <v>215</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>253</v>
+        <v>43</v>
       </c>
       <c r="AO38" t="s" s="2">
-        <v>254</v>
+        <v>43</v>
       </c>
       <c r="AP38" t="s" s="2">
         <v>43</v>
@@ -5577,18 +5746,18 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
         <v>44</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>43</v>
@@ -5597,18 +5766,20 @@
         <v>43</v>
       </c>
       <c r="I39" t="s" s="2">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>256</v>
+        <v>99</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>257</v>
+        <v>100</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>258</v>
-      </c>
-      <c r="M39" s="2"/>
+        <v>217</v>
+      </c>
+      <c r="M39" t="s" s="2">
+        <v>102</v>
+      </c>
       <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
         <v>43</v>
@@ -5657,13 +5828,13 @@
         <v>43</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>255</v>
+        <v>218</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="AH39" t="s" s="2">
         <v>43</v>
@@ -5678,7 +5849,7 @@
         <v>43</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>43</v>
+        <v>215</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>43</v>
@@ -5687,7 +5858,7 @@
         <v>43</v>
       </c>
       <c r="AO39" t="s" s="2">
-        <v>248</v>
+        <v>43</v>
       </c>
       <c r="AP39" t="s" s="2">
         <v>43</v>
@@ -5695,39 +5866,43 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
         <v>44</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>43</v>
       </c>
       <c r="H40" t="s" s="2">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="I40" t="s" s="2">
         <v>54</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>260</v>
+        <v>221</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>261</v>
-      </c>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
+        <v>222</v>
+      </c>
+      <c r="M40" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="N40" t="s" s="2">
+        <v>107</v>
+      </c>
       <c r="O40" t="s" s="2">
         <v>43</v>
       </c>
@@ -5775,13 +5950,13 @@
         <v>43</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>259</v>
+        <v>223</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="AH40" t="s" s="2">
         <v>43</v>
@@ -5796,13 +5971,13 @@
         <v>43</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AN40" t="s" s="2">
-        <v>262</v>
+        <v>43</v>
       </c>
       <c r="AO40" t="s" s="2">
         <v>43</v>
@@ -5813,7 +5988,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5821,10 +5996,10 @@
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>43</v>
@@ -5833,19 +6008,21 @@
         <v>43</v>
       </c>
       <c r="I41" t="s" s="2">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>264</v>
+        <v>133</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>265</v>
+        <v>281</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>266</v>
+        <v>282</v>
       </c>
       <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
+      <c r="N41" t="s" s="2">
+        <v>283</v>
+      </c>
       <c r="O41" t="s" s="2">
         <v>43</v>
       </c>
@@ -5869,13 +6046,13 @@
         <v>43</v>
       </c>
       <c r="W41" t="s" s="2">
-        <v>43</v>
+        <v>284</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>43</v>
+        <v>285</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>43</v>
+        <v>286</v>
       </c>
       <c r="Z41" t="s" s="2">
         <v>43</v>
@@ -5893,44 +6070,406 @@
         <v>43</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="AG41" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH41" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI41" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AJ41" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK41" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AL41" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM41" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AN41" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AO41" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AP41" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" hidden="true">
+      <c r="A42" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="F42" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="H42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="I42" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="J42" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="K42" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="L42" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="M42" s="2"/>
+      <c r="N42" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="O42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="P42" s="2"/>
+      <c r="Q42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="R42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="S42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="T42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="X42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Y42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE42" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="AF42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AG42" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AJ42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AL42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AN42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AO42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AP42" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" hidden="true">
+      <c r="A43" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="F43" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="H43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="I43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="J43" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="K43" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="M43" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="N43" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="O43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="P43" s="2"/>
+      <c r="Q43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="R43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="S43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="T43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="X43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Y43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE43" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="AF43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AG43" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AJ43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AL43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AN43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AO43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AP43" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" hidden="true">
+      <c r="A44" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="F44" t="s" s="2">
         <v>45</v>
       </c>
-      <c r="AH41" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI41" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AJ41" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK41" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL41" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM41" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AN41" t="s" s="2">
-        <v>142</v>
-      </c>
-      <c r="AO41" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="AP41" t="s" s="2">
-        <v>144</v>
+      <c r="G44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="H44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="I44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="J44" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="K44" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="L44" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="M44" s="2"/>
+      <c r="N44" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="O44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="P44" s="2"/>
+      <c r="Q44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="R44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="S44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="T44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="X44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Y44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE44" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="AF44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AG44" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AJ44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AL44" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="AM44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AN44" t="s" s="2">
+        <v>149</v>
+      </c>
+      <c r="AO44" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="AP44" t="s" s="2">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AP41">
+  <autoFilter ref="A1:AP44">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -5940,7 +6479,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI40">
+  <conditionalFormatting sqref="A2:AI43">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
update to latest changes
</commit_message>
<xml_diff>
--- a/docs/coverage-deqm.xlsx
+++ b/docs/coverage-deqm.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AP$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AP$41</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1689" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="268">
   <si>
     <t>Path</t>
   </si>
@@ -125,13 +125,13 @@
     <t>Mapping: Quality Data Model</t>
   </si>
   <si>
-    <t>Mapping: Workflow Pattern</t>
+    <t>Mapping: Workflow Mapping</t>
   </si>
   <si>
     <t>Mapping: RIM Mapping</t>
   </si>
   <si>
-    <t>Mapping: FiveWs Pattern Mapping</t>
+    <t>Mapping: W5 Mapping</t>
   </si>
   <si>
     <t>Mapping: Canadian Dental Association eclaims standard</t>
@@ -161,17 +161,17 @@
     <t>This is the Coverage profile which is used to provide insurance information for scheduling an appointment and or registering a patient.</t>
   </si>
   <si>
-    <t>The Coverage resource contains the insurance card level information, which is customary to provide on claims and other communications between providers and insurers.</t>
-  </si>
-  <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.div.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}</t>
+dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}</t>
   </si>
   <si>
     <t>Participation</t>
   </si>
   <si>
     <t>Event</t>
+  </si>
+  <si>
+    <t>financial.support</t>
   </si>
   <si>
     <t>Coverage.id</t>
@@ -212,7 +212,7 @@
     <t>Metadata about the resource</t>
   </si>
   <si>
-    <t>The metadata about the resource. This is content that is maintained by the infrastructure. Changes to the content might not always be associated with version changes to the resource.</t>
+    <t>The metadata about the resource. This is content that is maintained by the infrastructure. Changes to the content may not always be associated with version changes to the resource.</t>
   </si>
   <si>
     <t>Resource.meta</t>
@@ -228,10 +228,11 @@
     <t>A set of rules under which this content was created</t>
   </si>
   <si>
-    <t>A reference to a set of rules that were followed when the resource was constructed, and which must be understood when processing the content. Often, this is a reference to an implementation guide that defines the special rules along with other profiles etc.</t>
-  </si>
-  <si>
-    <t>Asserting this rule set restricts the content to be only understood by a limited set of trading partners. This inherently limits the usefulness of the data in the long term. However, the existing health eco-system is highly fractured, and not yet ready to define, collect, and exchange data in a generally computable sense. Wherever possible, implementers and/or specification writers should avoid using this element. Often, when used, the URL is a reference to an implementation guide that defines these special rules as part of it's narrative along with other profiles, value sets, etc.</t>
+    <t>A reference to a set of rules that were followed when the resource was constructed, and which must be understood when processing the content.</t>
+  </si>
+  <si>
+    <t>Asserting this rule set restricts the content to be only understood by a limited set of trading partners. This inherently limits the usefulness of the data in the long term. However, the existing health eco-system is highly fractured, and not yet ready to define, collect, and exchange data in a generally computable sense. Wherever possible, implementers and/or specification writers should avoid using this element. 
+This element is labelled as a modifier because the implicit rules may provide additional knowledge about the resource that modifies it's meaning or interpretation.</t>
   </si>
   <si>
     <t>Resource.implicitRules</t>
@@ -250,10 +251,10 @@
     <t>The base language in which the resource is written.</t>
   </si>
   <si>
-    <t>Language is provided to support indexing and accessibility (typically, services such as text to speech use the language tag). The html language tag in the narrative applies  to the narrative. The language tag on the resource may be used to specify the language of other presentations generated from the data in the resource. Not all the content has to be in the base language. The Resource.language should not be assumed to apply to the narrative automatically. If a language is specified, it should it also be specified on the div element in the html (see rules in HTML5 for information about the relationship between xml:lang and the html lang attribute).</t>
-  </si>
-  <si>
-    <t>preferred</t>
+    <t>Language is provided to support indexing and accessibility (typically, services such as text to speech use the language tag). The html language tag in the narrative applies  to the narrative. The language tag on the resource may be used to specify the language of other presentations generated from the data in the resource  Not all the content has to be in the base language. The Resource.language should not be assumed to apply to the narrative automatically. If a language is specified, it should it also be specified on the div element in the html (see rules in HTML5 for information about the relationship between xml:lang and the html lang attribute).</t>
+  </si>
+  <si>
+    <t>extensible</t>
   </si>
   <si>
     <t>A human language.</t>
@@ -279,13 +280,17 @@
     <t>Text summary of the resource, for human interpretation</t>
   </si>
   <si>
-    <t>A human-readable narrative that contains a summary of the resource and can be used to represent the content of the resource to a human. The narrative need not encode all the structured data, but is required to contain sufficient detail to make it "clinically safe" for a human to just read the narrative. Resource definitions may define what content should be represented in the narrative to ensure clinical safety.</t>
-  </si>
-  <si>
-    <t>Contained resources do not have narrative. Resources that are not contained SHOULD have a narrative. In some cases, a resource may only have text with little or no additional discrete data (as long as all minOccurs=1 elements are satisfied).  This may be necessary for data from legacy systems where information is captured as a "text blob" or where text is additionally entered raw or narrated and encoded information is added later.</t>
+    <t>A human-readable narrative that contains a summary of the resource, and may be used to represent the content of the resource to a human. The narrative need not encode all the structured data, but is required to contain sufficient detail to make it "clinically safe" for a human to just read the narrative. Resource definitions may define what content should be represented in the narrative to ensure clinical safety.</t>
+  </si>
+  <si>
+    <t>Contained resources do not have narrative. Resources that are not contained SHOULD have a narrative. In some cases, a resource may only have text with little or no additional discrete data (as long as all minOccurs=1 elements are satisfied).  This may be necessary for data from legacy systems where information is captured as a "text blob" or where text is additionally entered raw or narrated and encoded in formation is added later.</t>
   </si>
   <si>
     <t>DomainResource.text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dom-1
+</t>
   </si>
   <si>
     <t>Act.text?</t>
@@ -308,7 +313,7 @@
     <t>These resources do not have an independent existence apart from the resource that contains them - they cannot be identified independently, and nor can they have their own independent transaction scope.</t>
   </si>
   <si>
-    <t>This should never be done when the content can be identified properly, as once identification is lost, it is extremely difficult (and context dependent) to restore it again. Contained resources may have profiles and tags In their meta elements, but SHALL NOT have security labels.</t>
+    <t>This should never be done when the content can be identified properly, as once identification is lost, it is extremely difficult (and context dependent) to restore it again.</t>
   </si>
   <si>
     <t>DomainResource.contained</t>
@@ -328,10 +333,10 @@
 </t>
   </si>
   <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the resource. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+    <t>Additional Content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the resource. In order to make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
   </si>
   <si>
     <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
@@ -346,11 +351,7 @@
     <t>Extensions that cannot be ignored</t>
   </si>
   <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the resource and that modifies the understanding of the element that contains it and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
-Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
-  </si>
-  <si>
-    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
+    <t>May be used to represent additional information that is not part of the basic definition of the resource, and that modifies the understanding of the element that contains it. Usually modifier elements provide negation or qualification. In order to make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.</t>
   </si>
   <si>
     <t>DomainResource.modifierExtension</t>
@@ -363,27 +364,18 @@
 </t>
   </si>
   <si>
-    <t>Business Identifier for the coverage</t>
-  </si>
-  <si>
-    <t>A unique identifier assigned to this coverage.</t>
-  </si>
-  <si>
-    <t>The main (and possibly only) identifier for the coverage - often referred to as a Member Id, Certificate number, Personal Health Number or Case ID. May be constructed as the concatenation of the Coverage.SubscriberID and the Coverage.dependant.</t>
-  </si>
-  <si>
-    <t>Allows coverages to be distinguished and referenced.</t>
+    <t>The primary coverage ID</t>
+  </si>
+  <si>
+    <t>The main (and possibly only) identifier for the coverage - often referred to as a Member Id, Certificate number, Personal Health Number or Case ID. May be constructed as the concatination of the Coverage.SubscriberID and the Coverage.dependant.</t>
+  </si>
+  <si>
+    <t>This value may uniquely identify the coverage or it may be used in conjunction with the additional identifiers below.</t>
   </si>
   <si>
     <t>Event.identifier</t>
   </si>
   <si>
-    <t>.id</t>
-  </si>
-  <si>
-    <t>FiveWs.identifier</t>
-  </si>
-  <si>
     <t>C02</t>
   </si>
   <si>
@@ -405,25 +397,19 @@
     <t>This element is labeled as a modifier because the status contains the code entered-in-error that marks the coverage as not currently valid.</t>
   </si>
   <si>
-    <t>Need to track the status of the resource as 'draft' resources may undergo further edits while 'active' resources are immutable and may only have their status changed to 'cancelled'.</t>
-  </si>
-  <si>
     <t>required</t>
   </si>
   <si>
     <t>A code specifying the state of the resource instance.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/fm-status|4.0.0</t>
+    <t>http://hl7.org/fhir/ValueSet/fm-status</t>
   </si>
   <si>
     <t>Event.status</t>
   </si>
   <si>
-    <t>Act.status</t>
-  </si>
-  <si>
-    <t>FiveWs.status</t>
+    <t>status</t>
   </si>
   <si>
     <t>Coverage.type</t>
@@ -433,7 +419,7 @@
 </t>
   </si>
   <si>
-    <t>Coverage category such as medical or accident</t>
+    <t>Type of coverage such as medical or accident</t>
   </si>
   <si>
     <t>The type of coverage: social program, medical plan, accident coverage (workers compensation, auto), group health or payment by an individual or organization.</t>
@@ -451,7 +437,7 @@
     <t>code</t>
   </si>
   <si>
-    <t>FiveWs.class</t>
+    <t>class</t>
   </si>
   <si>
     <t>IN1-15</t>
@@ -467,16 +453,10 @@
     <t>Owner of the policy</t>
   </si>
   <si>
-    <t>The party who 'owns' the insurance policy.</t>
-  </si>
-  <si>
-    <t>For example: may be an individual, corporation or the subscriber's employer.</t>
-  </si>
-  <si>
-    <t>This provides employer information in the case of Worker's Compensation and other policies.</t>
-  </si>
-  <si>
-    <t>FiveWs.subject</t>
+    <t>The party who 'owns' the insurance policy,  may be an individual, corporation or the subscriber's employer.</t>
+  </si>
+  <si>
+    <t>who.focus</t>
   </si>
   <si>
     <t>D01 through D09</t>
@@ -501,12 +481,6 @@
     <t>The party who has signed-up for or 'owns' the contractual relationship to the policy or to whom the benefit of the policy for services rendered to them or their family is due.</t>
   </si>
   <si>
-    <t>May be self or a parent in the case of dependants.</t>
-  </si>
-  <si>
-    <t>This is the party who is entitled to the benfits under the policy.</t>
-  </si>
-  <si>
     <t>Coverage.subscriberId</t>
   </si>
   <si>
@@ -530,61 +504,37 @@
 </t>
   </si>
   <si>
-    <t>Plan beneficiary</t>
-  </si>
-  <si>
-    <t>The party who benefits from the insurance coverage; the patient when products and/or services are provided.</t>
-  </si>
-  <si>
-    <t>This is the party who receives treatment for which the costs are reimbursed under the coverage.</t>
+    <t>Plan Beneficiary</t>
+  </si>
+  <si>
+    <t>The party who benefits from the insurance coverage., the patient when services are provided.</t>
+  </si>
+  <si>
+    <t>While not required, this would usually be the US Core Patient Resource for which the MRP was performed.</t>
   </si>
   <si>
     <t>Event.subject</t>
   </si>
   <si>
-    <t>Coverage.dependent</t>
-  </si>
-  <si>
-    <t>Dependent number</t>
-  </si>
-  <si>
-    <t>A unique identifier for a dependent under the coverage.</t>
-  </si>
-  <si>
-    <t>Periodically the member number is constructed from the subscriberId and the dependant number.</t>
-  </si>
-  <si>
-    <t>For some coverages a single identifier is issued to the Subscriber and then a unique dependent number is issued to each beneficiary.</t>
-  </si>
-  <si>
-    <t>C17</t>
-  </si>
-  <si>
-    <t>- No exact HL7 v2 equivalent concept seems to exist;</t>
-  </si>
-  <si>
     <t>Coverage.relationship</t>
   </si>
   <si>
-    <t>Beneficiary relationship to the subscriber</t>
+    <t>Beneficiary relationship to the Subscriber</t>
   </si>
   <si>
     <t>The relationship of beneficiary (patient) to the subscriber.</t>
   </si>
   <si>
-    <t>Typically, an individual uses policies which are theirs (relationship='self') before policies owned by others.</t>
-  </si>
-  <si>
-    <t>To determine relationship between the patient and the subscriber to determine coordination of benefits.</t>
-  </si>
-  <si>
-    <t>extensible</t>
-  </si>
-  <si>
-    <t>The relationship between the Subscriber and the Beneficiary (insured/covered party/patient).</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/subscriber-relationship</t>
+    <t>To determine relationship between the patient and the subscriber.</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>The relationship between the Policyholder and the Beneficiary (insured/covered party/patient).</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/policyholder-relationship</t>
   </si>
   <si>
     <t>C03</t>
@@ -603,19 +553,13 @@
     <t>Time period during which the coverage is in force. A missing start date indicates the start date isn't known, a missing end date means the coverage is continuing to be in force.</t>
   </si>
   <si>
-    <t>Some insurers require the submission of the coverage term.</t>
-  </si>
-  <si>
     <t>participationPeriod</t>
   </si>
   <si>
-    <t>Event.occurrence[x]</t>
-  </si>
-  <si>
-    <t>Act.effectiveTime</t>
-  </si>
-  <si>
-    <t>FiveWs.done[x]</t>
+    <t>Event.occurrence</t>
+  </si>
+  <si>
+    <t>when.done</t>
   </si>
   <si>
     <t>IN1-12 / IN1-13</t>
@@ -624,20 +568,16 @@
     <t>Coverage.payor</t>
   </si>
   <si>
-    <t>Issuer of the policy</t>
-  </si>
-  <si>
-    <t>The program or plan underwriter or payor including both insurance and non-insurance agreements, such as patient-pay agreements.</t>
-  </si>
-  <si>
-    <t>May provide multiple identifiers such as insurance company identifier or business identifier (BIN number).
-For selfpay it may provide multiple paying persons and/or organizations.</t>
-  </si>
-  <si>
-    <t>Need to identify the issuer to target for claim processing and for coordination of benefit processing.</t>
-  </si>
-  <si>
-    <t>FiveWs.author</t>
+    <t>Identifier for the plan or agreement issuer</t>
+  </si>
+  <si>
+    <t>The program or plan underwriter or payor including both insurance and non-insurance agreements, such as patient-pay agreements. May provide multiple identifiers such as insurance company identifier or business identifier (BIN number).</t>
+  </si>
+  <si>
+    <t>Need to identify the issuer to target for processing and for coordination of benefit processing.</t>
+  </si>
+  <si>
+    <t>who.author</t>
   </si>
   <si>
     <t>A05</t>
@@ -649,7 +589,7 @@
     <t>C.30</t>
   </si>
   <si>
-    <t>Coverage.class</t>
+    <t>Coverage.grouping</t>
   </si>
   <si>
     <t xml:space="preserve">BackboneElement
@@ -659,26 +599,20 @@
     <t>Additional coverage classifications</t>
   </si>
   <si>
-    <t>A suite of underwriter specific classifiers.</t>
-  </si>
-  <si>
-    <t>For example may be used to identify a class of coverage or employer group, Policy, Plan.</t>
-  </si>
-  <si>
-    <t>The codes provided on the health card which identify or confirm the specific policy for the insurer.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+    <t>A suite of underwrite specific classifiers, for example may be used to identify a class of coverage or employer group, Policy, Plan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
 </t>
   </si>
   <si>
-    <t>Coverage.class.id</t>
-  </si>
-  <si>
-    <t>Unique id for inter-element referencing</t>
-  </si>
-  <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+    <t>Coverage.grouping.id</t>
+  </si>
+  <si>
+    <t>xml:id (or equivalent in JSON)</t>
+  </si>
+  <si>
+    <t>unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
   </si>
   <si>
     <t>Element.id</t>
@@ -687,63 +621,35 @@
     <t>n/a</t>
   </si>
   <si>
-    <t>Coverage.class.extension</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+    <t>Coverage.grouping.extension</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. In order to make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
   </si>
   <si>
     <t>Element.extension</t>
   </si>
   <si>
-    <t>Coverage.class.modifierExtension</t>
+    <t>Coverage.grouping.modifierExtension</t>
   </si>
   <si>
     <t>extensions
 user contentmodifiers</t>
   </si>
   <si>
-    <t>Extensions that cannot be ignored even if unrecognized</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element and that modifies the understanding of the element in which it is contained and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
-Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
+    <t>May be used to represent additional information that is not part of the basic definition of the element, and that modifies the understanding of the element that contains it. Usually modifier elements provide negation or qualification. In order to make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.</t>
   </si>
   <si>
     <t>BackboneElement.modifierExtension</t>
   </si>
   <si>
-    <t>Coverage.class.type</t>
-  </si>
-  <si>
-    <t>Type of class such as 'group' or 'plan'</t>
-  </si>
-  <si>
-    <t>The type of classification for which an insurer-specific class label or number and optional name is provided, for example may be used to identify a class of coverage or employer group, Policy, Plan.</t>
-  </si>
-  <si>
-    <t>The insurer issued label for a specific health card value.</t>
-  </si>
-  <si>
-    <t>The policy classifications, eg. Group, Plan, Class, etc.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/coverage-class</t>
-  </si>
-  <si>
-    <t>Coverage.class.value</t>
-  </si>
-  <si>
-    <t>Value associated with the type</t>
-  </si>
-  <si>
-    <t>The alphanumeric string value associated with the insurer issued label.</t>
-  </si>
-  <si>
-    <t>For example, the Group or Plan number.</t>
-  </si>
-  <si>
-    <t>The insurer issued label and value are necessary to identify the specific policy.</t>
+    <t>Coverage.grouping.group</t>
+  </si>
+  <si>
+    <t>An identifier for the group</t>
+  </si>
+  <si>
+    <t>Identifies a style or collective of coverage issued by the underwriter, for example may be used to identify an employer group. May also be referred to as a Policy or Group ID.</t>
   </si>
   <si>
     <t>C11 (Division,Section)</t>
@@ -755,16 +661,148 @@
     <t>C.31</t>
   </si>
   <si>
-    <t>Coverage.class.name</t>
-  </si>
-  <si>
-    <t>Human readable description of the type and value</t>
+    <t>Coverage.grouping.groupDisplay</t>
+  </si>
+  <si>
+    <t>Display text for an identifier for the group</t>
+  </si>
+  <si>
+    <t>A short description for the group.</t>
+  </si>
+  <si>
+    <t>Coverage.grouping.subGroup</t>
+  </si>
+  <si>
+    <t>An identifier for the subsection of the group</t>
+  </si>
+  <si>
+    <t>Identifies a style or collective of coverage issued by the underwriter, for example may be used to identify a subset of an employer group.</t>
+  </si>
+  <si>
+    <t>Coverage.grouping.subGroupDisplay</t>
+  </si>
+  <si>
+    <t>Display text for the subsection of the group</t>
+  </si>
+  <si>
+    <t>A short description for the subgroup.</t>
+  </si>
+  <si>
+    <t>Coverage.grouping.plan</t>
+  </si>
+  <si>
+    <t>An identifier for the plan</t>
+  </si>
+  <si>
+    <t>Identifies a style or collective of coverage issued by the underwriter, for example may be used to identify a collection of benefits provided to employees. May be referred to as a Section or Division ID.</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>IN1-35</t>
+  </si>
+  <si>
+    <t>Coverage.grouping.planDisplay</t>
+  </si>
+  <si>
+    <t>Display text for the plan</t>
+  </si>
+  <si>
+    <t>A short description for the plan.</t>
+  </si>
+  <si>
+    <t>Coverage.grouping.subPlan</t>
+  </si>
+  <si>
+    <t>An identifier for the subsection of the plan</t>
+  </si>
+  <si>
+    <t>Identifies a sub-style or sub-collective of coverage issued by the underwriter, for example may be used to identify a subset of a collection of benefits provided to employees.</t>
+  </si>
+  <si>
+    <t>IN1-10</t>
+  </si>
+  <si>
+    <t>Coverage.grouping.subPlanDisplay</t>
+  </si>
+  <si>
+    <t>Display text for the subsection of the plan</t>
+  </si>
+  <si>
+    <t>A short description for the subplan.</t>
+  </si>
+  <si>
+    <t>Coverage.grouping.class</t>
+  </si>
+  <si>
+    <t>An identifier for the class</t>
+  </si>
+  <si>
+    <t>Identifies a style or collective of coverage issues by the underwriter, for example may be used to identify a class of coverage such as a level of deductables or co-payment.</t>
+  </si>
+  <si>
+    <t>Coverage.grouping.classDisplay</t>
+  </si>
+  <si>
+    <t>Display text for the class</t>
   </si>
   <si>
     <t>A short description for the class.</t>
   </si>
   <si>
-    <t>Used to provide a meaningful description in correspondence to the patient.</t>
+    <t>Coverage.grouping.subClass</t>
+  </si>
+  <si>
+    <t>An identifier for the subsection of the class</t>
+  </si>
+  <si>
+    <t>Identifies a sub-style or sub-collective of coverage issues by the underwriter, for example may be used to identify a subclass of coverage such as a sub-level of deductables or co-payment.</t>
+  </si>
+  <si>
+    <t>Coverage.grouping.subClassDisplay</t>
+  </si>
+  <si>
+    <t>Display text for the subsection of the subclass</t>
+  </si>
+  <si>
+    <t>A short description for the subclass.</t>
+  </si>
+  <si>
+    <t>Coverage.dependent</t>
+  </si>
+  <si>
+    <t>Dependent number</t>
+  </si>
+  <si>
+    <t>A unique identifier for a dependent under the coverage.</t>
+  </si>
+  <si>
+    <t>For some coverage a single identifier is issued to the Subscriber and a dependent number issued to each beneficiary.</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>- No exact HL7 v2 equivalent concept seems to exist;</t>
+  </si>
+  <si>
+    <t>Coverage.sequence</t>
+  </si>
+  <si>
+    <t>The plan instance or sequence counter</t>
+  </si>
+  <si>
+    <t>An optional counter for a particular instance of the identified coverage which increments upon each renewal.</t>
+  </si>
+  <si>
+    <t>Some coverage, for example social plans, may be offered in short time increments, for example for a week or a month at a time, so while the rest of the plan details and identifiers may remain constant over time, the instance is incremented with each renewal and provided to the covered party on their 'card'.</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>No HL7 v2 equivalent concept seems to exist</t>
   </si>
   <si>
     <t>Coverage.order</t>
@@ -777,10 +815,7 @@
     <t>Relative order of the coverage</t>
   </si>
   <si>
-    <t>The order of applicability of this coverage relative to other coverages which are currently in force. Note, there may be gaps in the numbering and this does not imply primary, secondary etc. as the specific positioning of coverages depends upon the episode of care.</t>
-  </si>
-  <si>
-    <t>Used in managing the coordination of benefits.</t>
+    <t>The order of applicability of this coverage relative to other coverages which are currently inforce. Note, there may be gaps in the numbering and this does not imply primary, secondard etc. as the specific positioning of coverages depends upon the episode of care.</t>
   </si>
   <si>
     <t>Coverage.network</t>
@@ -792,148 +827,7 @@
     <t>The insurer-specific identifier for the insurer-defined network of providers to which the beneficiary may seek treatment which will be covered at the 'in-network' rate, otherwise 'out of network' terms and conditions apply.</t>
   </si>
   <si>
-    <t>Used in referral for treatment and in claims processing.</t>
-  </si>
-  <si>
     <t>D10</t>
-  </si>
-  <si>
-    <t>Coverage.costToBeneficiary</t>
-  </si>
-  <si>
-    <t>CoPay
-DeductibleExceptions</t>
-  </si>
-  <si>
-    <t>Patient payments for services/products</t>
-  </si>
-  <si>
-    <t>A suite of codes indicating the cost category and associated amount which have been detailed in the policy and may have been  included on the health card.</t>
-  </si>
-  <si>
-    <t>For example by knowing the patient visit co-pay, the provider can collect the amount prior to undertaking treatment.</t>
-  </si>
-  <si>
-    <t>Required by providers to manage financial transaction with the patient.</t>
-  </si>
-  <si>
-    <t>Coverage.costToBeneficiary.id</t>
-  </si>
-  <si>
-    <t>Coverage.costToBeneficiary.extension</t>
-  </si>
-  <si>
-    <t>Coverage.costToBeneficiary.modifierExtension</t>
-  </si>
-  <si>
-    <t>Coverage.costToBeneficiary.type</t>
-  </si>
-  <si>
-    <t>Cost category</t>
-  </si>
-  <si>
-    <t>The category of patient centric costs associated with treatment.</t>
-  </si>
-  <si>
-    <t>For example visit, specialist visits, emergency, inpatient care, etc.</t>
-  </si>
-  <si>
-    <t>Needed to identify the category associated with the amount for the patient.</t>
-  </si>
-  <si>
-    <t>The types of services to which patient copayments are specified.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/coverage-copay-type</t>
-  </si>
-  <si>
-    <t>Coverage.costToBeneficiary.value[x]</t>
-  </si>
-  <si>
-    <t>Quantity {SimpleQuantity}
-Money</t>
-  </si>
-  <si>
-    <t>The amount or percentage due from the beneficiary</t>
-  </si>
-  <si>
-    <t>The amount due from the patient for the cost category.</t>
-  </si>
-  <si>
-    <t>Amount may be expressed as a percentage of the service/product cost or a fixed amount of currency.</t>
-  </si>
-  <si>
-    <t>Needed to identify the amount for the patient associated with the category.</t>
-  </si>
-  <si>
-    <t>Coverage.costToBeneficiary.exception</t>
-  </si>
-  <si>
-    <t>Exceptions for patient payments</t>
-  </si>
-  <si>
-    <t>A suite of codes indicating exceptions or reductions to patient costs and their effective periods.</t>
-  </si>
-  <si>
-    <t>Coverage.costToBeneficiary.exception.id</t>
-  </si>
-  <si>
-    <t>Coverage.costToBeneficiary.exception.extension</t>
-  </si>
-  <si>
-    <t>Coverage.costToBeneficiary.exception.modifierExtension</t>
-  </si>
-  <si>
-    <t>Coverage.costToBeneficiary.exception.type</t>
-  </si>
-  <si>
-    <t>Exception category</t>
-  </si>
-  <si>
-    <t>The code for the specific exception.</t>
-  </si>
-  <si>
-    <t>Needed to identify the exception associated with the amount for the patient.</t>
-  </si>
-  <si>
-    <t>example</t>
-  </si>
-  <si>
-    <t>The types of exceptions from the part or full value of financial obligations such as copays.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/coverage-financial-exception</t>
-  </si>
-  <si>
-    <t>Coverage.costToBeneficiary.exception.period</t>
-  </si>
-  <si>
-    <t>The effective period of the exception</t>
-  </si>
-  <si>
-    <t>The timeframe during when the exception is in force.</t>
-  </si>
-  <si>
-    <t>Needed to identify the applicable timeframe for the exception for the correct calculation of patient costs.</t>
-  </si>
-  <si>
-    <t>Coverage.subrogation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boolean
-</t>
-  </si>
-  <si>
-    <t>Reimbursement to insurer</t>
-  </si>
-  <si>
-    <t>When 'subrogation=true' this insurance instance has been included not for adjudication but to provide insurers with the details to recover costs.</t>
-  </si>
-  <si>
-    <t>Typically, automotive and worker's compensation policies would be flagged with 'subrogation=true' to enable healthcare payors to collect against accident claims.</t>
-  </si>
-  <si>
-    <t>See definition for when to be used.</t>
   </si>
   <si>
     <t>Coverage.contract</t>
@@ -947,9 +841,6 @@
   </si>
   <si>
     <t>The policy(s) which constitute this insurance coverage.</t>
-  </si>
-  <si>
-    <t>To reference the legally binding contract between the policy holder and the insurer.</t>
   </si>
   <si>
     <t>IN1-16, 18,  19</t>
@@ -1101,7 +992,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AP44"/>
+  <dimension ref="A1:AP41"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1110,7 +1001,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="51.6015625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="34.8046875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.45703125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
@@ -1140,15 +1031,15 @@
     <col min="28" max="28" width="18.84375" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="41.1484375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="31" max="31" width="33.828125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="28.43359375" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="26.6875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="28.0703125" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="22.67578125" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="33.046875" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="22.0078125" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="54.171875" customWidth="true" bestFit="true"/>
     <col min="41" max="41" width="50.94140625" customWidth="true" bestFit="true"/>
     <col min="42" max="42" width="57.1640625" customWidth="true" bestFit="true"/>
@@ -1315,9 +1206,7 @@
       <c r="L2" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="M2" t="s" s="2">
-        <v>48</v>
-      </c>
+      <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" t="s" s="2">
         <v>43</v>
@@ -1378,19 +1267,19 @@
         <v>43</v>
       </c>
       <c r="AI2" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AJ2" t="s" s="2">
         <v>49</v>
       </c>
-      <c r="AJ2" t="s" s="2">
+      <c r="AK2" t="s" s="2">
         <v>50</v>
-      </c>
-      <c r="AK2" t="s" s="2">
-        <v>51</v>
       </c>
       <c r="AL2" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AM2" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AN2" t="s" s="2">
         <v>43</v>
@@ -1973,7 +1862,7 @@
         <v>53</v>
       </c>
       <c r="AH7" t="s" s="2">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="AI7" t="s" s="2">
         <v>43</v>
@@ -1985,7 +1874,7 @@
         <v>43</v>
       </c>
       <c r="AL7" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AM7" t="s" s="2">
         <v>43</v>
@@ -2002,11 +1891,11 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" t="s" s="2">
@@ -2025,16 +1914,16 @@
         <v>43</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -2084,7 +1973,7 @@
         <v>43</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>44</v>
@@ -2105,7 +1994,7 @@
         <v>43</v>
       </c>
       <c r="AL8" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AM8" t="s" s="2">
         <v>43</v>
@@ -2122,11 +2011,11 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
@@ -2145,16 +2034,16 @@
         <v>43</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
@@ -2204,7 +2093,7 @@
         <v>43</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>44</v>
@@ -2225,7 +2114,7 @@
         <v>43</v>
       </c>
       <c r="AL9" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AM9" t="s" s="2">
         <v>43</v>
@@ -2242,11 +2131,11 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
@@ -2265,20 +2154,18 @@
         <v>43</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="N10" t="s" s="2">
-        <v>107</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
         <v>43</v>
       </c>
@@ -2347,7 +2234,7 @@
         <v>43</v>
       </c>
       <c r="AL10" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AM10" t="s" s="2">
         <v>43</v>
@@ -2395,11 +2282,9 @@
       <c r="L11" t="s" s="2">
         <v>112</v>
       </c>
-      <c r="M11" t="s" s="2">
+      <c r="M11" s="2"/>
+      <c r="N11" t="s" s="2">
         <v>113</v>
-      </c>
-      <c r="N11" t="s" s="2">
-        <v>114</v>
       </c>
       <c r="O11" t="s" s="2">
         <v>43</v>
@@ -2466,27 +2351,27 @@
         <v>43</v>
       </c>
       <c r="AK11" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="AL11" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM11" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AN11" t="s" s="2">
         <v>115</v>
       </c>
-      <c r="AL11" t="s" s="2">
+      <c r="AO11" t="s" s="2">
         <v>116</v>
       </c>
-      <c r="AM11" t="s" s="2">
+      <c r="AP11" t="s" s="2">
         <v>117</v>
-      </c>
-      <c r="AN11" t="s" s="2">
-        <v>118</v>
-      </c>
-      <c r="AO11" t="s" s="2">
-        <v>119</v>
-      </c>
-      <c r="AP11" t="s" s="2">
-        <v>120</v>
       </c>
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -2494,7 +2379,7 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s" s="2">
         <v>53</v>
@@ -2512,17 +2397,15 @@
         <v>73</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>124</v>
-      </c>
-      <c r="N12" t="s" s="2">
-        <v>125</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
         <v>43</v>
       </c>
@@ -2546,55 +2429,55 @@
         <v>43</v>
       </c>
       <c r="W12" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="X12" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="Y12" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="Z12" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA12" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB12" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC12" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD12" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE12" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="AF12" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AG12" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH12" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI12" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AJ12" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK12" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AL12" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM12" t="s" s="2">
         <v>126</v>
-      </c>
-      <c r="X12" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="Y12" t="s" s="2">
-        <v>128</v>
-      </c>
-      <c r="Z12" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA12" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB12" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC12" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD12" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE12" t="s" s="2">
-        <v>121</v>
-      </c>
-      <c r="AF12" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AG12" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AH12" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI12" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AJ12" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK12" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="AL12" t="s" s="2">
-        <v>130</v>
-      </c>
-      <c r="AM12" t="s" s="2">
-        <v>131</v>
       </c>
       <c r="AN12" t="s" s="2">
         <v>43</v>
@@ -2608,7 +2491,7 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -2631,17 +2514,17 @@
         <v>54</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" t="s" s="2">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="O13" t="s" s="2">
         <v>43</v>
@@ -2666,13 +2549,13 @@
         <v>43</v>
       </c>
       <c r="W13" t="s" s="2">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="X13" t="s" s="2">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="Y13" t="s" s="2">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>43</v>
@@ -2690,7 +2573,7 @@
         <v>43</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>44</v>
@@ -2705,7 +2588,7 @@
         <v>43</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="AK13" t="s" s="2">
         <v>43</v>
@@ -2714,13 +2597,13 @@
         <v>43</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="AN13" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AO13" t="s" s="2">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="AP13" t="s" s="2">
         <v>43</v>
@@ -2728,7 +2611,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -2751,20 +2634,16 @@
         <v>54</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="M14" t="s" s="2">
-        <v>146</v>
-      </c>
-      <c r="N14" t="s" s="2">
-        <v>147</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
         <v>43</v>
       </c>
@@ -2812,45 +2691,45 @@
         <v>43</v>
       </c>
       <c r="AE14" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="AF14" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AG14" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH14" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI14" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AJ14" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK14" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AL14" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM14" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="AN14" t="s" s="2">
         <v>142</v>
       </c>
-      <c r="AF14" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG14" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AH14" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI14" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AJ14" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK14" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL14" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM14" t="s" s="2">
-        <v>148</v>
-      </c>
-      <c r="AN14" t="s" s="2">
-        <v>149</v>
-      </c>
       <c r="AO14" t="s" s="2">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="AP14" t="s" s="2">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -2873,20 +2752,16 @@
         <v>54</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="M15" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="N15" t="s" s="2">
-        <v>157</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
         <v>43</v>
       </c>
@@ -2934,7 +2809,7 @@
         <v>43</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>44</v>
@@ -2958,21 +2833,21 @@
         <v>43</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="AO15" t="s" s="2">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="AP15" t="s" s="2">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2995,17 +2870,17 @@
         <v>54</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" t="s" s="2">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="O16" t="s" s="2">
         <v>43</v>
@@ -3054,7 +2929,7 @@
         <v>43</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>44</v>
@@ -3078,21 +2953,21 @@
         <v>43</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="AO16" t="s" s="2">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="AP16" t="s" s="2">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3100,7 +2975,7 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F17" t="s" s="2">
         <v>53</v>
@@ -3115,17 +2990,17 @@
         <v>54</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" t="s" s="2">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>43</v>
@@ -3174,10 +3049,10 @@
         <v>43</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>53</v>
@@ -3192,27 +3067,27 @@
         <v>43</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="AL17" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="AO17" t="s" s="2">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="AP17" t="s" s="2">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3232,22 +3107,20 @@
         <v>43</v>
       </c>
       <c r="I18" t="s" s="2">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>171</v>
-      </c>
-      <c r="M18" t="s" s="2">
-        <v>172</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="M18" s="2"/>
       <c r="N18" t="s" s="2">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="O18" t="s" s="2">
         <v>43</v>
@@ -3272,13 +3145,13 @@
         <v>43</v>
       </c>
       <c r="W18" t="s" s="2">
-        <v>43</v>
+        <v>164</v>
       </c>
       <c r="X18" t="s" s="2">
-        <v>43</v>
+        <v>165</v>
       </c>
       <c r="Y18" t="s" s="2">
-        <v>43</v>
+        <v>166</v>
       </c>
       <c r="Z18" t="s" s="2">
         <v>43</v>
@@ -3296,7 +3169,7 @@
         <v>43</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>44</v>
@@ -3323,10 +3196,10 @@
         <v>43</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="AO18" t="s" s="2">
-        <v>175</v>
+        <v>43</v>
       </c>
       <c r="AP18" t="s" s="2">
         <v>43</v>
@@ -3334,7 +3207,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3354,23 +3227,19 @@
         <v>43</v>
       </c>
       <c r="I19" t="s" s="2">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>133</v>
+        <v>169</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>178</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>179</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>180</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
         <v>43</v>
       </c>
@@ -3394,13 +3263,13 @@
         <v>43</v>
       </c>
       <c r="W19" t="s" s="2">
-        <v>181</v>
+        <v>43</v>
       </c>
       <c r="X19" t="s" s="2">
-        <v>182</v>
+        <v>43</v>
       </c>
       <c r="Y19" t="s" s="2">
-        <v>183</v>
+        <v>43</v>
       </c>
       <c r="Z19" t="s" s="2">
         <v>43</v>
@@ -3418,45 +3287,45 @@
         <v>43</v>
       </c>
       <c r="AE19" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="AF19" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AG19" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH19" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI19" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AJ19" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="AK19" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="AL19" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM19" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="AN19" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AO19" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="AP19" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="2">
         <v>176</v>
-      </c>
-      <c r="AF19" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG19" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AH19" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI19" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AJ19" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK19" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL19" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM19" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AN19" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="AO19" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AP19" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" hidden="true">
-      <c r="A20" t="s" s="2">
-        <v>185</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3467,10 +3336,10 @@
         <v>44</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>43</v>
@@ -3479,17 +3348,17 @@
         <v>54</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>186</v>
+        <v>138</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" t="s" s="2">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>43</v>
@@ -3538,13 +3407,13 @@
         <v>43</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG20" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="AH20" t="s" s="2">
         <v>43</v>
@@ -3553,30 +3422,30 @@
         <v>43</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>190</v>
+        <v>43</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>191</v>
+        <v>43</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>192</v>
+        <v>43</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>43</v>
+        <v>181</v>
       </c>
       <c r="AO20" t="s" s="2">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="AP20" t="s" s="2">
-        <v>43</v>
+        <v>183</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3584,35 +3453,31 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F21" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>43</v>
       </c>
       <c r="I21" t="s" s="2">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>143</v>
+        <v>185</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>197</v>
-      </c>
-      <c r="M21" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="N21" t="s" s="2">
-        <v>199</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
         <v>43</v>
       </c>
@@ -3660,19 +3525,19 @@
         <v>43</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="AG21" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="AH21" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>43</v>
+        <v>188</v>
       </c>
       <c r="AJ21" t="s" s="2">
         <v>43</v>
@@ -3684,21 +3549,21 @@
         <v>43</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>200</v>
+        <v>43</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>201</v>
+        <v>43</v>
       </c>
       <c r="AO21" t="s" s="2">
-        <v>202</v>
+        <v>43</v>
       </c>
       <c r="AP21" t="s" s="2">
-        <v>203</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3709,7 +3574,7 @@
         <v>44</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G22" t="s" s="2">
         <v>43</v>
@@ -3721,20 +3586,16 @@
         <v>43</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>205</v>
+        <v>150</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>207</v>
-      </c>
-      <c r="M22" t="s" s="2">
-        <v>208</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>209</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
         <v>43</v>
       </c>
@@ -3782,19 +3643,19 @@
         <v>43</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="AH22" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>210</v>
+        <v>43</v>
       </c>
       <c r="AJ22" t="s" s="2">
         <v>43</v>
@@ -3803,7 +3664,7 @@
         <v>43</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>43</v>
+        <v>193</v>
       </c>
       <c r="AM22" t="s" s="2">
         <v>43</v>
@@ -3820,18 +3681,18 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
         <v>44</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>43</v>
@@ -3843,15 +3704,17 @@
         <v>43</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>159</v>
+        <v>100</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>212</v>
+        <v>101</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>213</v>
-      </c>
-      <c r="M23" s="2"/>
+        <v>195</v>
+      </c>
+      <c r="M23" t="s" s="2">
+        <v>103</v>
+      </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
         <v>43</v>
@@ -3900,13 +3763,13 @@
         <v>43</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="AH23" t="s" s="2">
         <v>43</v>
@@ -3921,7 +3784,7 @@
         <v>43</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="AM23" t="s" s="2">
         <v>43</v>
@@ -3938,11 +3801,11 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>98</v>
+        <v>198</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
@@ -3955,22 +3818,22 @@
         <v>43</v>
       </c>
       <c r="H24" t="s" s="2">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
@@ -4020,7 +3883,7 @@
         <v>43</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>44</v>
@@ -4041,7 +3904,7 @@
         <v>43</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>215</v>
+        <v>97</v>
       </c>
       <c r="AM24" t="s" s="2">
         <v>43</v>
@@ -4058,43 +3921,39 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
-        <v>220</v>
+        <v>43</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
         <v>44</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G25" t="s" s="2">
         <v>43</v>
       </c>
       <c r="H25" t="s" s="2">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="I25" t="s" s="2">
         <v>54</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>99</v>
+        <v>150</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="M25" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="N25" t="s" s="2">
-        <v>107</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
         <v>43</v>
       </c>
@@ -4142,13 +4001,13 @@
         <v>43</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>223</v>
+        <v>201</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG25" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="AH25" t="s" s="2">
         <v>43</v>
@@ -4163,24 +4022,24 @@
         <v>43</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>96</v>
+        <v>43</v>
       </c>
       <c r="AM25" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>43</v>
+        <v>204</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>43</v>
+        <v>205</v>
       </c>
       <c r="AP25" t="s" s="2">
-        <v>43</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4188,7 +4047,7 @@
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F26" t="s" s="2">
         <v>53</v>
@@ -4203,18 +4062,16 @@
         <v>54</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="M26" s="2"/>
-      <c r="N26" t="s" s="2">
-        <v>227</v>
-      </c>
+      <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
         <v>43</v>
       </c>
@@ -4238,13 +4095,13 @@
         <v>43</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>181</v>
+        <v>43</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>228</v>
+        <v>43</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>229</v>
+        <v>43</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>43</v>
@@ -4262,10 +4119,10 @@
         <v>43</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>53</v>
@@ -4289,18 +4146,18 @@
         <v>43</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>43</v>
+        <v>204</v>
       </c>
       <c r="AO26" t="s" s="2">
-        <v>43</v>
+        <v>205</v>
       </c>
       <c r="AP26" t="s" s="2">
-        <v>43</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4308,7 +4165,7 @@
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F27" t="s" s="2">
         <v>53</v>
@@ -4323,20 +4180,16 @@
         <v>54</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="M27" t="s" s="2">
-        <v>233</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>234</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
         <v>43</v>
       </c>
@@ -4384,10 +4237,10 @@
         <v>43</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>53</v>
@@ -4411,18 +4264,18 @@
         <v>43</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>235</v>
+        <v>43</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>236</v>
+        <v>205</v>
       </c>
       <c r="AP27" t="s" s="2">
-        <v>237</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4445,18 +4298,16 @@
         <v>54</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>239</v>
+        <v>214</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="M28" s="2"/>
-      <c r="N28" t="s" s="2">
-        <v>241</v>
-      </c>
+      <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
         <v>43</v>
       </c>
@@ -4504,7 +4355,7 @@
         <v>43</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>44</v>
@@ -4531,18 +4382,18 @@
         <v>43</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>235</v>
+        <v>43</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>236</v>
+        <v>205</v>
       </c>
       <c r="AP28" t="s" s="2">
-        <v>237</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4565,18 +4416,16 @@
         <v>54</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>243</v>
+        <v>150</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>244</v>
+        <v>217</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="M29" s="2"/>
-      <c r="N29" t="s" s="2">
-        <v>246</v>
-      </c>
+      <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
         <v>43</v>
       </c>
@@ -4624,7 +4473,7 @@
         <v>43</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>44</v>
@@ -4651,10 +4500,10 @@
         <v>43</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>43</v>
+        <v>219</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>175</v>
+        <v>220</v>
       </c>
       <c r="AP29" t="s" s="2">
         <v>43</v>
@@ -4662,7 +4511,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>247</v>
+        <v>221</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4685,18 +4534,16 @@
         <v>54</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>248</v>
+        <v>222</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="M30" s="2"/>
-      <c r="N30" t="s" s="2">
-        <v>250</v>
-      </c>
+      <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
         <v>43</v>
       </c>
@@ -4744,7 +4591,7 @@
         <v>43</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>247</v>
+        <v>221</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>44</v>
@@ -4771,10 +4618,10 @@
         <v>43</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>251</v>
+        <v>219</v>
       </c>
       <c r="AO30" t="s" s="2">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="AP30" t="s" s="2">
         <v>43</v>
@@ -4782,18 +4629,18 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>252</v>
+        <v>224</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>253</v>
+        <v>43</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
         <v>44</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>43</v>
@@ -4802,23 +4649,19 @@
         <v>43</v>
       </c>
       <c r="I31" t="s" s="2">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>205</v>
+        <v>150</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>254</v>
+        <v>225</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>255</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>257</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
         <v>43</v>
       </c>
@@ -4866,19 +4709,19 @@
         <v>43</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>252</v>
+        <v>224</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG31" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="AH31" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>210</v>
+        <v>43</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>43</v>
@@ -4896,7 +4739,7 @@
         <v>43</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>43</v>
+        <v>227</v>
       </c>
       <c r="AP31" t="s" s="2">
         <v>43</v>
@@ -4904,7 +4747,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>258</v>
+        <v>228</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4924,16 +4767,16 @@
         <v>43</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>213</v>
+        <v>230</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -4984,7 +4827,7 @@
         <v>43</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>44</v>
@@ -5005,7 +4848,7 @@
         <v>43</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>215</v>
+        <v>43</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>43</v>
@@ -5014,7 +4857,7 @@
         <v>43</v>
       </c>
       <c r="AO32" t="s" s="2">
-        <v>43</v>
+        <v>227</v>
       </c>
       <c r="AP32" t="s" s="2">
         <v>43</v>
@@ -5022,18 +4865,18 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>259</v>
+        <v>231</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
         <v>44</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>43</v>
@@ -5042,20 +4885,18 @@
         <v>43</v>
       </c>
       <c r="I33" t="s" s="2">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>99</v>
+        <v>150</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>100</v>
+        <v>232</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>102</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>43</v>
@@ -5104,13 +4945,13 @@
         <v>43</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="AH33" t="s" s="2">
         <v>43</v>
@@ -5125,16 +4966,16 @@
         <v>43</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>215</v>
+        <v>43</v>
       </c>
       <c r="AM33" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>43</v>
+        <v>219</v>
       </c>
       <c r="AO33" t="s" s="2">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="AP33" t="s" s="2">
         <v>43</v>
@@ -5142,43 +4983,39 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>260</v>
+        <v>234</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>220</v>
+        <v>43</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
         <v>44</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G34" t="s" s="2">
         <v>43</v>
       </c>
       <c r="H34" t="s" s="2">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="I34" t="s" s="2">
         <v>54</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>99</v>
+        <v>150</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="N34" t="s" s="2">
-        <v>107</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
         <v>43</v>
       </c>
@@ -5226,13 +5063,13 @@
         <v>43</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG34" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="AH34" t="s" s="2">
         <v>43</v>
@@ -5247,16 +5084,16 @@
         <v>43</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>96</v>
+        <v>43</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>43</v>
+        <v>219</v>
       </c>
       <c r="AO34" t="s" s="2">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="AP34" t="s" s="2">
         <v>43</v>
@@ -5264,7 +5101,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>261</v>
+        <v>237</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5287,20 +5124,16 @@
         <v>54</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>263</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>265</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
         <v>43</v>
       </c>
@@ -5324,13 +5157,13 @@
         <v>43</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>181</v>
+        <v>43</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>266</v>
+        <v>43</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>267</v>
+        <v>43</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>43</v>
@@ -5348,7 +5181,7 @@
         <v>43</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>261</v>
+        <v>237</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>44</v>
@@ -5375,10 +5208,10 @@
         <v>43</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>43</v>
+        <v>219</v>
       </c>
       <c r="AO35" t="s" s="2">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="AP35" t="s" s="2">
         <v>43</v>
@@ -5386,7 +5219,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5394,7 +5227,7 @@
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F36" t="s" s="2">
         <v>53</v>
@@ -5409,20 +5242,16 @@
         <v>54</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>269</v>
+        <v>150</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>270</v>
+        <v>241</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="N36" t="s" s="2">
-        <v>273</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
         <v>43</v>
       </c>
@@ -5470,10 +5299,10 @@
         <v>43</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>53</v>
@@ -5497,18 +5326,18 @@
         <v>43</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="AO36" t="s" s="2">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="AP36" t="s" s="2">
-        <v>237</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>274</v>
+        <v>243</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5519,7 +5348,7 @@
         <v>44</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>43</v>
@@ -5528,20 +5357,20 @@
         <v>43</v>
       </c>
       <c r="I37" t="s" s="2">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>205</v>
+        <v>150</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>275</v>
+        <v>244</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" t="s" s="2">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>43</v>
@@ -5590,19 +5419,19 @@
         <v>43</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>274</v>
+        <v>243</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="AH37" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>210</v>
+        <v>43</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>43</v>
@@ -5617,10 +5446,10 @@
         <v>43</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>43</v>
+        <v>247</v>
       </c>
       <c r="AO37" t="s" s="2">
-        <v>43</v>
+        <v>248</v>
       </c>
       <c r="AP37" t="s" s="2">
         <v>43</v>
@@ -5628,7 +5457,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>277</v>
+        <v>249</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5648,19 +5477,21 @@
         <v>43</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>212</v>
+        <v>250</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
+      <c r="N38" t="s" s="2">
+        <v>252</v>
+      </c>
       <c r="O38" t="s" s="2">
         <v>43</v>
       </c>
@@ -5708,7 +5539,7 @@
         <v>43</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>214</v>
+        <v>249</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>44</v>
@@ -5729,16 +5560,16 @@
         <v>43</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>215</v>
+        <v>43</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>43</v>
+        <v>253</v>
       </c>
       <c r="AO38" t="s" s="2">
-        <v>43</v>
+        <v>254</v>
       </c>
       <c r="AP38" t="s" s="2">
         <v>43</v>
@@ -5746,18 +5577,18 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>278</v>
+        <v>255</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
         <v>44</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>43</v>
@@ -5766,20 +5597,18 @@
         <v>43</v>
       </c>
       <c r="I39" t="s" s="2">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>99</v>
+        <v>256</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>100</v>
+        <v>257</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>102</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
         <v>43</v>
@@ -5828,13 +5657,13 @@
         <v>43</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>218</v>
+        <v>255</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="AH39" t="s" s="2">
         <v>43</v>
@@ -5849,7 +5678,7 @@
         <v>43</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>215</v>
+        <v>43</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>43</v>
@@ -5858,7 +5687,7 @@
         <v>43</v>
       </c>
       <c r="AO39" t="s" s="2">
-        <v>43</v>
+        <v>248</v>
       </c>
       <c r="AP39" t="s" s="2">
         <v>43</v>
@@ -5866,43 +5695,39 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>279</v>
+        <v>259</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>220</v>
+        <v>43</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
         <v>44</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>43</v>
       </c>
       <c r="H40" t="s" s="2">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="I40" t="s" s="2">
         <v>54</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>99</v>
+        <v>150</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>221</v>
+        <v>260</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>107</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
         <v>43</v>
       </c>
@@ -5950,13 +5775,13 @@
         <v>43</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>223</v>
+        <v>259</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="AH40" t="s" s="2">
         <v>43</v>
@@ -5971,13 +5796,13 @@
         <v>43</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>96</v>
+        <v>43</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AN40" t="s" s="2">
-        <v>43</v>
+        <v>262</v>
       </c>
       <c r="AO40" t="s" s="2">
         <v>43</v>
@@ -5988,7 +5813,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5996,10 +5821,10 @@
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>43</v>
@@ -6008,21 +5833,19 @@
         <v>43</v>
       </c>
       <c r="I41" t="s" s="2">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>133</v>
+        <v>264</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>281</v>
+        <v>265</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="M41" s="2"/>
-      <c r="N41" t="s" s="2">
-        <v>283</v>
-      </c>
+      <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>43</v>
       </c>
@@ -6046,13 +5869,13 @@
         <v>43</v>
       </c>
       <c r="W41" t="s" s="2">
-        <v>284</v>
+        <v>43</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>285</v>
+        <v>43</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>286</v>
+        <v>43</v>
       </c>
       <c r="Z41" t="s" s="2">
         <v>43</v>
@@ -6070,13 +5893,13 @@
         <v>43</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>43</v>
@@ -6097,379 +5920,17 @@
         <v>43</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>43</v>
+        <v>142</v>
       </c>
       <c r="AO41" t="s" s="2">
-        <v>43</v>
+        <v>267</v>
       </c>
       <c r="AP41" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="42" hidden="true">
-      <c r="A42" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="B42" s="2"/>
-      <c r="C42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D42" s="2"/>
-      <c r="E42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F42" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="G42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I42" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="J42" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="K42" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="L42" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="M42" s="2"/>
-      <c r="N42" t="s" s="2">
-        <v>290</v>
-      </c>
-      <c r="O42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P42" s="2"/>
-      <c r="Q42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="T42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE42" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="AF42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG42" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AH42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AJ42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AN42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AO42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AP42" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" hidden="true">
-      <c r="A43" t="s" s="2">
-        <v>291</v>
-      </c>
-      <c r="B43" s="2"/>
-      <c r="C43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D43" s="2"/>
-      <c r="E43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F43" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="G43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="J43" t="s" s="2">
-        <v>292</v>
-      </c>
-      <c r="K43" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="L43" t="s" s="2">
-        <v>294</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>295</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>296</v>
-      </c>
-      <c r="O43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P43" s="2"/>
-      <c r="Q43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="T43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE43" t="s" s="2">
-        <v>291</v>
-      </c>
-      <c r="AF43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG43" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AH43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AJ43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AN43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AO43" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AP43" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" hidden="true">
-      <c r="A44" t="s" s="2">
-        <v>297</v>
-      </c>
-      <c r="B44" s="2"/>
-      <c r="C44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D44" s="2"/>
-      <c r="E44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F44" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="G44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="J44" t="s" s="2">
-        <v>298</v>
-      </c>
-      <c r="K44" t="s" s="2">
-        <v>299</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>300</v>
-      </c>
-      <c r="M44" s="2"/>
-      <c r="N44" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="O44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P44" s="2"/>
-      <c r="Q44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="T44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE44" t="s" s="2">
-        <v>297</v>
-      </c>
-      <c r="AF44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG44" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AJ44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL44" t="s" s="2">
-        <v>215</v>
-      </c>
-      <c r="AM44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AN44" t="s" s="2">
-        <v>149</v>
-      </c>
-      <c r="AO44" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="AP44" t="s" s="2">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AP44">
+  <autoFilter ref="A1:AP41">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -6479,7 +5940,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI43">
+  <conditionalFormatting sqref="A2:AI40">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>